<commit_message>
Added S(8) & actual slack
</commit_message>
<xml_diff>
--- a/results/Strategies by Year Comparison.xlsx
+++ b/results/Strategies by Year Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5C25AB-5A93-C148-A5F8-344F38B192A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8545739B-1ED9-EF47-9C4A-CC20EE4AD228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Strategy 8</t>
+  </si>
+  <si>
+    <t>slack</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,18 +443,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,13 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BCF68F-9CA1-1A41-B9FD-C7E5B292FD92}">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AD19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -790,10 +784,12 @@
     <col min="22" max="23" width="5.83203125" customWidth="1"/>
     <col min="24" max="24" width="5.83203125" style="1" customWidth="1"/>
     <col min="25" max="26" width="5.83203125" customWidth="1"/>
-    <col min="27" max="27" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.83203125" style="1" customWidth="1"/>
+    <col min="28" max="29" width="5.83203125" customWidth="1"/>
+    <col min="30" max="30" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="6" t="s">
@@ -835,10 +831,15 @@
       <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="2"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -912,16 +913,25 @@
         <v>8</v>
       </c>
       <c r="Y2" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z2" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23">
         <v>2000</v>
       </c>
@@ -992,20 +1002,29 @@
       <c r="W3" s="25">
         <v>600</v>
       </c>
-      <c r="X3" s="47">
+      <c r="X3" s="26">
         <v>89</v>
       </c>
       <c r="Y3" s="25">
         <v>165</v>
       </c>
-      <c r="Z3" s="27">
-        <v>600</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="Z3" s="25">
+        <v>600</v>
+      </c>
+      <c r="AA3" s="26">
+        <v>91</v>
+      </c>
+      <c r="AB3" s="25">
+        <v>-2</v>
+      </c>
+      <c r="AC3" s="27">
+        <v>-3</v>
+      </c>
+      <c r="AD3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2002</v>
       </c>
@@ -1073,23 +1092,32 @@
       <c r="V4">
         <v>165</v>
       </c>
-      <c r="W4" s="35">
-        <v>600</v>
-      </c>
-      <c r="X4" s="39">
+      <c r="W4">
+        <v>600</v>
+      </c>
+      <c r="X4" s="1">
         <v>84</v>
       </c>
       <c r="Y4">
         <v>165</v>
       </c>
-      <c r="Z4" s="12">
-        <v>600</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="Z4" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>85</v>
+      </c>
+      <c r="AB4">
+        <v>-1</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>9</v>
+      </c>
+      <c r="AD4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2004</v>
       </c>
@@ -1157,353 +1185,400 @@
       <c r="V5">
         <v>165</v>
       </c>
-      <c r="W5" s="35">
-        <v>600</v>
-      </c>
-      <c r="X5" s="39">
+      <c r="W5">
+        <v>600</v>
+      </c>
+      <c r="X5" s="1">
         <v>93</v>
       </c>
       <c r="Y5">
         <v>165</v>
       </c>
-      <c r="Z5" s="12">
-        <v>600</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="Z5" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>94</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>4</v>
+      </c>
+      <c r="AD5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
         <v>2006</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="3">
         <v>0.54039999999999999</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6">
         <v>233</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6">
         <v>435</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="1">
         <v>167</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6">
         <v>306</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6">
         <v>741</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="38">
+      <c r="J6">
         <v>4</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6">
         <v>439</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="1">
         <v>5</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6">
         <v>6</v>
       </c>
-      <c r="N6" s="38">
+      <c r="N6">
         <v>441</v>
       </c>
-      <c r="O6" s="39">
+      <c r="O6" s="1">
         <v>4</v>
       </c>
-      <c r="P6" s="38">
+      <c r="P6">
         <v>4</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6">
         <f t="shared" si="0"/>
         <v>439</v>
       </c>
-      <c r="R6" s="39">
+      <c r="R6" s="1">
         <v>30</v>
       </c>
-      <c r="S6" s="38">
+      <c r="S6">
         <v>50</v>
       </c>
-      <c r="T6" s="38">
+      <c r="T6">
         <v>485</v>
       </c>
-      <c r="U6" s="39">
+      <c r="U6" s="1">
         <v>92</v>
       </c>
-      <c r="V6" s="38">
+      <c r="V6">
         <v>165</v>
       </c>
-      <c r="W6" s="40">
-        <v>600</v>
-      </c>
-      <c r="X6" s="39">
+      <c r="W6">
+        <v>600</v>
+      </c>
+      <c r="X6" s="1">
         <v>92</v>
       </c>
-      <c r="Y6" s="38">
+      <c r="Y6">
         <v>165</v>
       </c>
-      <c r="Z6" s="41">
-        <v>600</v>
-      </c>
-      <c r="AA6" s="38" t="s">
+      <c r="Z6" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>89</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>-21</v>
+      </c>
+      <c r="AD6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
         <v>2008</v>
       </c>
-      <c r="B7" s="37">
+      <c r="B7" s="3">
         <v>0.55289999999999995</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7">
         <v>257</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7">
         <v>435</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7">
         <v>-16</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="1">
         <v>57</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7">
         <v>132</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7">
         <v>567</v>
       </c>
-      <c r="I7" s="39">
+      <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7">
         <v>29</v>
       </c>
-      <c r="K7" s="38">
+      <c r="K7">
         <v>464</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="1">
         <v>9</v>
       </c>
-      <c r="M7" s="38">
+      <c r="M7">
         <v>46</v>
       </c>
-      <c r="N7" s="38">
+      <c r="N7">
         <v>481</v>
       </c>
-      <c r="O7" s="39">
+      <c r="O7" s="1">
         <v>15</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7">
         <v>57</v>
       </c>
-      <c r="Q7" s="38">
+      <c r="Q7">
         <f t="shared" si="0"/>
         <v>492</v>
       </c>
-      <c r="R7" s="39">
+      <c r="R7" s="1">
         <v>12</v>
       </c>
-      <c r="S7" s="38">
+      <c r="S7">
         <v>50</v>
       </c>
-      <c r="T7" s="38">
+      <c r="T7">
         <v>485</v>
       </c>
-      <c r="U7" s="39">
+      <c r="U7" s="1">
         <v>75</v>
       </c>
-      <c r="V7" s="38">
+      <c r="V7">
         <v>165</v>
       </c>
-      <c r="W7" s="40">
-        <v>600</v>
-      </c>
-      <c r="X7" s="39">
+      <c r="W7">
+        <v>600</v>
+      </c>
+      <c r="X7" s="1">
         <v>75</v>
       </c>
-      <c r="Y7" s="38">
+      <c r="Y7">
         <v>165</v>
       </c>
-      <c r="Z7" s="41">
-        <v>600</v>
-      </c>
-      <c r="AA7" s="38" t="s">
+      <c r="Z7" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB7">
+        <v>-2</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>-33</v>
+      </c>
+      <c r="AD7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
         <v>2010</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="29">
         <v>0.4723</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="30">
         <v>193</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="30">
         <v>435</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="30">
         <v>12</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="31">
         <v>54</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="30">
         <v>89</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="30">
         <v>524</v>
       </c>
-      <c r="I8" s="45">
+      <c r="I8" s="31">
         <v>23</v>
       </c>
-      <c r="J8" s="44">
+      <c r="J8" s="30">
         <v>23</v>
       </c>
-      <c r="K8" s="44">
+      <c r="K8" s="30">
         <v>458</v>
       </c>
-      <c r="L8" s="45">
+      <c r="L8" s="31">
         <v>29</v>
       </c>
-      <c r="M8" s="44">
+      <c r="M8" s="30">
         <v>36</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="30">
         <v>471</v>
       </c>
-      <c r="O8" s="45">
+      <c r="O8" s="31">
         <v>28</v>
       </c>
-      <c r="P8" s="44">
+      <c r="P8" s="30">
         <v>33</v>
       </c>
-      <c r="Q8" s="44">
+      <c r="Q8" s="30">
         <f t="shared" si="0"/>
         <v>468</v>
       </c>
-      <c r="R8" s="45">
+      <c r="R8" s="31">
         <v>36</v>
       </c>
-      <c r="S8" s="44">
+      <c r="S8" s="30">
         <v>50</v>
       </c>
-      <c r="T8" s="44">
+      <c r="T8" s="30">
         <v>485</v>
       </c>
-      <c r="U8" s="45">
+      <c r="U8" s="31">
         <v>90</v>
       </c>
-      <c r="V8" s="44">
+      <c r="V8" s="30">
         <v>165</v>
       </c>
-      <c r="W8" s="44">
-        <v>600</v>
-      </c>
-      <c r="X8" s="45">
+      <c r="W8" s="30">
+        <v>600</v>
+      </c>
+      <c r="X8" s="31">
         <v>90</v>
       </c>
-      <c r="Y8" s="44">
+      <c r="Y8" s="30">
         <v>165</v>
       </c>
-      <c r="Z8" s="46">
-        <v>600</v>
-      </c>
+      <c r="Z8" s="30">
+        <v>600</v>
+      </c>
+      <c r="AA8" s="31">
+        <v>95</v>
+      </c>
+      <c r="AB8" s="30">
+        <v>-5</v>
+      </c>
+      <c r="AC8" s="32">
+        <v>11</v>
+      </c>
+      <c r="AD8"/>
     </row>
-    <row r="9" spans="1:27" s="38" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
         <v>2012</v>
       </c>
-      <c r="B9" s="37">
+      <c r="B9" s="3">
         <v>0.50849999999999995</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9">
         <v>201</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9">
         <v>435</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9">
         <v>20</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="1">
         <v>106</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9">
         <v>169</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9">
         <v>604</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="1">
         <v>41</v>
       </c>
-      <c r="J9" s="38">
+      <c r="J9">
         <v>41</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9">
         <v>476</v>
       </c>
-      <c r="L9" s="39">
+      <c r="L9" s="1">
         <v>54</v>
       </c>
-      <c r="M9" s="38">
+      <c r="M9">
         <v>67</v>
       </c>
-      <c r="N9" s="38">
+      <c r="N9">
         <v>502</v>
       </c>
-      <c r="O9" s="39">
+      <c r="O9" s="1">
         <v>44</v>
       </c>
-      <c r="P9" s="38">
+      <c r="P9">
         <v>47</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9">
         <f t="shared" si="0"/>
         <v>482</v>
       </c>
-      <c r="R9" s="39">
+      <c r="R9" s="1">
         <v>46</v>
       </c>
-      <c r="S9" s="38">
+      <c r="S9">
         <v>50</v>
       </c>
-      <c r="T9" s="38">
+      <c r="T9">
         <v>485</v>
       </c>
-      <c r="U9" s="39">
+      <c r="U9" s="1">
         <v>105</v>
       </c>
-      <c r="V9" s="38">
+      <c r="V9">
         <v>165</v>
       </c>
-      <c r="W9" s="40">
-        <v>600</v>
-      </c>
-      <c r="X9" s="39">
+      <c r="W9">
+        <v>600</v>
+      </c>
+      <c r="X9" s="1">
         <v>105</v>
       </c>
-      <c r="Y9" s="38">
+      <c r="Y9">
         <v>165</v>
       </c>
-      <c r="Z9" s="41">
-        <v>600</v>
-      </c>
+      <c r="Z9" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>102</v>
+      </c>
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="12">
+        <v>-2</v>
+      </c>
+      <c r="AD9"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2014</v>
       </c>
@@ -1571,21 +1646,30 @@
       <c r="V10">
         <v>165</v>
       </c>
-      <c r="W10" s="35">
-        <v>600</v>
-      </c>
-      <c r="X10" s="39">
+      <c r="W10">
+        <v>600</v>
+      </c>
+      <c r="X10" s="1">
         <v>96</v>
       </c>
       <c r="Y10">
         <v>165</v>
       </c>
-      <c r="Z10" s="12">
-        <v>600</v>
-      </c>
-      <c r="AA10"/>
+      <c r="Z10" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>95</v>
+      </c>
+      <c r="AB10">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="12">
+        <v>16</v>
+      </c>
+      <c r="AD10"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>2016</v>
       </c>
@@ -1653,21 +1737,30 @@
       <c r="V11">
         <v>165</v>
       </c>
-      <c r="W11" s="35">
-        <v>600</v>
-      </c>
-      <c r="X11" s="39">
+      <c r="W11">
+        <v>600</v>
+      </c>
+      <c r="X11" s="1">
         <v>103</v>
       </c>
       <c r="Y11">
         <v>165</v>
       </c>
-      <c r="Z11" s="12">
-        <v>600</v>
-      </c>
-      <c r="AA11"/>
+      <c r="Z11" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>101</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="12">
+        <v>4</v>
+      </c>
+      <c r="AD11"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>2018</v>
       </c>
@@ -1735,23 +1828,32 @@
       <c r="V12">
         <v>165</v>
       </c>
-      <c r="W12" s="35">
-        <v>600</v>
-      </c>
-      <c r="X12" s="39">
+      <c r="W12">
+        <v>600</v>
+      </c>
+      <c r="X12" s="1">
         <v>85</v>
       </c>
       <c r="Y12">
         <v>165</v>
       </c>
-      <c r="Z12" s="12">
-        <v>600</v>
-      </c>
-      <c r="AA12" t="s">
+      <c r="Z12" s="35">
+        <v>600</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>85</v>
+      </c>
+      <c r="AB12">
+        <v>-1</v>
+      </c>
+      <c r="AC12" s="12">
+        <v>-20</v>
+      </c>
+      <c r="AD12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>2020</v>
       </c>
@@ -1822,18 +1924,27 @@
       <c r="W13" s="30">
         <v>600</v>
       </c>
-      <c r="X13" s="45">
+      <c r="X13" s="31">
         <v>83</v>
       </c>
       <c r="Y13" s="30">
         <v>165</v>
       </c>
-      <c r="Z13" s="32">
-        <v>600</v>
-      </c>
-      <c r="AA13"/>
+      <c r="Z13" s="30">
+        <v>600</v>
+      </c>
+      <c r="AA13" s="31">
+        <v>84</v>
+      </c>
+      <c r="AB13" s="30">
+        <v>-2</v>
+      </c>
+      <c r="AC13" s="32">
+        <v>-5</v>
+      </c>
+      <c r="AD13"/>
     </row>
-    <row r="14" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>2022</v>
       </c>
@@ -1861,10 +1972,13 @@
       <c r="W14" s="15"/>
       <c r="X14" s="16"/>
       <c r="Y14" s="15"/>
-      <c r="Z14" s="17"/>
-      <c r="AA14"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>14</v>
       </c>
@@ -1914,8 +2028,15 @@
         <f>MIN(Z$3:Z$14)</f>
         <v>600</v>
       </c>
+      <c r="AB16" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC16">
+        <f>MIN(AC$3:AC$14)</f>
+        <v>-33</v>
+      </c>
     </row>
-    <row r="17" spans="7:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:29" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
         <v>15</v>
       </c>
@@ -1965,8 +2086,15 @@
         <f>MAX(Z$3:Z$14)</f>
         <v>600</v>
       </c>
+      <c r="AB17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC17">
+        <f>MAX(AC$3:AC$14)</f>
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="7:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:29" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>16</v>
       </c>
@@ -2017,8 +2145,15 @@
         <f>AVERAGE(Z$3:Z$14)</f>
         <v>600</v>
       </c>
+      <c r="AB18" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC18" s="33">
+        <f>AVERAGE(AC$3:AC$14)</f>
+        <v>-3.6363636363636362</v>
+      </c>
     </row>
-    <row r="19" spans="7:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:29" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
         <v>17</v>
       </c>
@@ -2068,6 +2203,13 @@
       <c r="Z19" s="33">
         <f>STDEV(Z$3:Z$14)</f>
         <v>0</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC19" s="33">
+        <f>STDEV(AC$3:AC$14)</f>
+        <v>15.207055778635963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-ran S(7) w/ slack
</commit_message>
<xml_diff>
--- a/results/Strategies by Year Comparison.xlsx
+++ b/results/Strategies by Year Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8545739B-1ED9-EF47-9C4A-CC20EE4AD228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D149A4-8610-7944-892B-E5B963C4AFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="500" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
@@ -763,7 +763,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="Z14" sqref="Z14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1006,10 +1006,10 @@
         <v>89</v>
       </c>
       <c r="Y3" s="25">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z3" s="25">
-        <v>600</v>
+        <v>-1</v>
       </c>
       <c r="AA3" s="26">
         <v>91</v>
@@ -1099,10 +1099,10 @@
         <v>84</v>
       </c>
       <c r="Y4">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="35">
-        <v>600</v>
+        <v>10</v>
       </c>
       <c r="AA4" s="1">
         <v>85</v>
@@ -1192,10 +1192,10 @@
         <v>93</v>
       </c>
       <c r="Y5">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="35">
-        <v>600</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="1">
         <v>94</v>
@@ -1285,10 +1285,10 @@
         <v>92</v>
       </c>
       <c r="Y6">
-        <v>165</v>
+        <v>-1</v>
       </c>
       <c r="Z6" s="35">
-        <v>600</v>
+        <v>-24</v>
       </c>
       <c r="AA6" s="1">
         <v>89</v>
@@ -1378,10 +1378,10 @@
         <v>75</v>
       </c>
       <c r="Y7">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="35">
-        <v>600</v>
+        <v>-31</v>
       </c>
       <c r="AA7" s="1">
         <v>77</v>
@@ -1471,10 +1471,10 @@
         <v>90</v>
       </c>
       <c r="Y8" s="30">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z8" s="30">
-        <v>600</v>
+        <v>16</v>
       </c>
       <c r="AA8" s="31">
         <v>95</v>
@@ -1562,10 +1562,10 @@
         <v>105</v>
       </c>
       <c r="Y9">
-        <v>165</v>
+        <v>-1</v>
       </c>
       <c r="Z9" s="35">
-        <v>600</v>
+        <v>-5</v>
       </c>
       <c r="AA9" s="1">
         <v>102</v>
@@ -1653,10 +1653,10 @@
         <v>96</v>
       </c>
       <c r="Y10">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="35">
-        <v>600</v>
+        <v>15</v>
       </c>
       <c r="AA10" s="1">
         <v>95</v>
@@ -1744,10 +1744,10 @@
         <v>103</v>
       </c>
       <c r="Y11">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="Z11" s="35">
-        <v>600</v>
+        <v>2</v>
       </c>
       <c r="AA11" s="1">
         <v>101</v>
@@ -1835,10 +1835,10 @@
         <v>85</v>
       </c>
       <c r="Y12">
-        <v>165</v>
+        <v>-1</v>
       </c>
       <c r="Z12" s="35">
-        <v>600</v>
+        <v>-20</v>
       </c>
       <c r="AA12" s="1">
         <v>85</v>
@@ -1928,10 +1928,10 @@
         <v>83</v>
       </c>
       <c r="Y13" s="30">
-        <v>165</v>
+        <v>-1</v>
       </c>
       <c r="Z13" s="30">
-        <v>600</v>
+        <v>-4</v>
       </c>
       <c r="AA13" s="31">
         <v>84</v>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="Z16">
         <f>MIN(Z$3:Z$14)</f>
-        <v>600</v>
+        <v>-31</v>
       </c>
       <c r="AB16" t="s">
         <v>14</v>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="Z17">
         <f>MAX(Z$3:Z$14)</f>
-        <v>600</v>
+        <v>16</v>
       </c>
       <c r="AB17" t="s">
         <v>15</v>
@@ -2143,7 +2143,7 @@
       </c>
       <c r="Z18" s="33">
         <f>AVERAGE(Z$3:Z$14)</f>
-        <v>600</v>
+        <v>-3.3636363636363638</v>
       </c>
       <c r="AB18" t="s">
         <v>16</v>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="Z19" s="33">
         <f>STDEV(Z$3:Z$14)</f>
-        <v>0</v>
+        <v>15.698870833742962</v>
       </c>
       <c r="AB19" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Analyzed preliminary 2022 election results
</commit_message>
<xml_diff>
--- a/results/Strategies by Year Comparison.xlsx
+++ b/results/Strategies by Year Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E01A8-369D-9142-99AE-FBDB8FD0E11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82C58FD-900E-AF4B-9C97-C1C960ADC831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="5400" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
+    <workbookView xWindow="19820" yWindow="11300" windowWidth="27680" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategies" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t>Year</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>slack</t>
+  </si>
+  <si>
+    <t>Preliminary</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -450,6 +452,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,7 +773,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -847,91 +850,91 @@
       <c r="AD1" s="2"/>
     </row>
     <row r="2" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="V2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="W2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="Y2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="Z2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AA2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AB2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" s="22" t="s">
+      <c r="AC2" s="21" t="s">
         <v>25</v>
       </c>
       <c r="AD2" s="2" t="s">
@@ -939,92 +942,92 @@
       </c>
     </row>
     <row r="3" spans="1:30" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36">
+      <c r="A3" s="35">
         <v>2000</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>0.503</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>212</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>433</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="24">
         <v>23</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>35</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <v>470</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="24">
         <v>11</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="23">
         <v>11</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="23">
         <v>446</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="24">
         <v>12</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="23">
         <v>13</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="23">
         <v>448</v>
       </c>
-      <c r="O3" s="25">
+      <c r="O3" s="24">
         <v>11</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="23">
         <v>11</v>
       </c>
-      <c r="Q3" s="24">
+      <c r="Q3" s="23">
         <f>435+P3</f>
         <v>446</v>
       </c>
-      <c r="R3" s="25">
+      <c r="R3" s="24">
         <v>31</v>
       </c>
-      <c r="S3" s="24">
+      <c r="S3" s="23">
         <v>50</v>
       </c>
-      <c r="T3" s="24">
+      <c r="T3" s="23">
         <v>485</v>
       </c>
-      <c r="U3" s="25">
+      <c r="U3" s="24">
         <v>89</v>
       </c>
-      <c r="V3" s="24">
+      <c r="V3" s="23">
         <v>165</v>
       </c>
-      <c r="W3" s="24">
+      <c r="W3" s="23">
         <v>600</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="24">
         <v>89</v>
       </c>
-      <c r="Y3" s="24">
+      <c r="Y3" s="23">
         <v>0</v>
       </c>
-      <c r="Z3" s="24">
+      <c r="Z3" s="23">
         <v>-1</v>
       </c>
-      <c r="AA3" s="25">
+      <c r="AA3" s="24">
         <v>91</v>
       </c>
-      <c r="AB3" s="24">
+      <c r="AB3" s="23">
         <v>-2</v>
       </c>
-      <c r="AC3" s="26">
+      <c r="AC3" s="25">
         <v>-3</v>
       </c>
       <c r="AD3" t="s">
@@ -1081,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q13" si="0">435+P4</f>
+        <f t="shared" ref="Q4:Q14" si="0">435+P4</f>
         <v>445</v>
       </c>
       <c r="R4" s="1">
@@ -1404,98 +1407,98 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="27">
+      <c r="A8" s="26">
         <v>2010</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>0.4723</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>193</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="28">
         <v>435</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="28">
         <v>12</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <v>54</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <v>89</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="28">
         <v>524</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>23</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="28">
         <v>23</v>
       </c>
-      <c r="K8" s="29">
+      <c r="K8" s="28">
         <v>458</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="29">
         <v>29</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="28">
         <v>36</v>
       </c>
-      <c r="N8" s="29">
+      <c r="N8" s="28">
         <v>471</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="29">
         <v>28</v>
       </c>
-      <c r="P8" s="29">
+      <c r="P8" s="28">
         <v>33</v>
       </c>
-      <c r="Q8" s="29">
+      <c r="Q8" s="28">
         <f t="shared" si="0"/>
         <v>468</v>
       </c>
-      <c r="R8" s="30">
+      <c r="R8" s="29">
         <v>36</v>
       </c>
-      <c r="S8" s="29">
+      <c r="S8" s="28">
         <v>50</v>
       </c>
-      <c r="T8" s="29">
+      <c r="T8" s="28">
         <v>485</v>
       </c>
-      <c r="U8" s="30">
+      <c r="U8" s="29">
         <v>90</v>
       </c>
-      <c r="V8" s="29">
+      <c r="V8" s="28">
         <v>165</v>
       </c>
-      <c r="W8" s="29">
+      <c r="W8" s="28">
         <v>600</v>
       </c>
-      <c r="X8" s="30">
+      <c r="X8" s="29">
         <v>90</v>
       </c>
-      <c r="Y8" s="29">
+      <c r="Y8" s="28">
         <v>0</v>
       </c>
-      <c r="Z8" s="29">
+      <c r="Z8" s="28">
         <v>16</v>
       </c>
-      <c r="AA8" s="30">
+      <c r="AA8" s="29">
         <v>95</v>
       </c>
-      <c r="AB8" s="29">
+      <c r="AB8" s="28">
         <v>-5</v>
       </c>
-      <c r="AC8" s="31">
+      <c r="AC8" s="30">
         <v>11</v>
       </c>
       <c r="AD8"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>2012</v>
       </c>
       <c r="B9" s="3">
@@ -1861,129 +1864,188 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="27">
+      <c r="A13" s="26">
         <v>2020</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="27">
         <v>0.50680000000000003</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C13" s="28">
         <v>222</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="28">
         <v>435</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E13" s="28">
         <v>-2</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="29">
         <v>6</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="28">
         <v>14</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="28">
         <v>449</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="29">
         <v>0</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="28">
         <v>3</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="28">
         <v>438</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="29">
         <v>4</v>
       </c>
-      <c r="M13" s="29">
+      <c r="M13" s="28">
         <v>10</v>
       </c>
-      <c r="N13" s="29">
+      <c r="N13" s="28">
         <v>445</v>
       </c>
-      <c r="O13" s="30">
+      <c r="O13" s="29">
         <v>1</v>
       </c>
-      <c r="P13" s="29">
+      <c r="P13" s="28">
         <v>5</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="Q13" s="28">
         <f t="shared" si="0"/>
         <v>440</v>
       </c>
-      <c r="R13" s="30">
+      <c r="R13" s="29">
         <v>24</v>
       </c>
-      <c r="S13" s="29">
+      <c r="S13" s="28">
         <v>50</v>
       </c>
-      <c r="T13" s="29">
+      <c r="T13" s="28">
         <v>485</v>
       </c>
-      <c r="U13" s="30">
+      <c r="U13" s="29">
         <v>83</v>
       </c>
-      <c r="V13" s="29">
+      <c r="V13" s="28">
         <v>165</v>
       </c>
-      <c r="W13" s="29">
+      <c r="W13" s="28">
         <v>600</v>
       </c>
-      <c r="X13" s="30">
+      <c r="X13" s="29">
         <v>83</v>
       </c>
-      <c r="Y13" s="29">
+      <c r="Y13" s="28">
         <v>-1</v>
       </c>
-      <c r="Z13" s="29">
+      <c r="Z13" s="28">
         <v>-4</v>
       </c>
-      <c r="AA13" s="30">
+      <c r="AA13" s="29">
         <v>84</v>
       </c>
-      <c r="AB13" s="29">
+      <c r="AB13" s="28">
         <v>-2</v>
       </c>
-      <c r="AC13" s="31">
+      <c r="AC13" s="30">
         <v>-5</v>
       </c>
       <c r="AD13"/>
     </row>
     <row r="14" spans="1:30" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="36">
         <v>2022</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="17"/>
-      <c r="AD14"/>
+      <c r="B14" s="13">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="C14" s="14">
+        <v>213</v>
+      </c>
+      <c r="D14" s="14">
+        <v>435</v>
+      </c>
+      <c r="E14" s="14">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14">
+        <v>436</v>
+      </c>
+      <c r="I14" s="15">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="14">
+        <v>436</v>
+      </c>
+      <c r="L14" s="15">
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="14">
+        <v>436</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
+      <c r="P14" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="14">
+        <f t="shared" si="0"/>
+        <v>436</v>
+      </c>
+      <c r="R14" s="15">
+        <v>23</v>
+      </c>
+      <c r="S14" s="14">
+        <v>50</v>
+      </c>
+      <c r="T14" s="14">
+        <v>485</v>
+      </c>
+      <c r="U14" s="15">
+        <v>79</v>
+      </c>
+      <c r="V14" s="14">
+        <v>165</v>
+      </c>
+      <c r="W14" s="14">
+        <v>600</v>
+      </c>
+      <c r="X14" s="15">
+        <v>79</v>
+      </c>
+      <c r="Y14" s="14">
+        <v>165</v>
+      </c>
+      <c r="Z14" s="14">
+        <v>600</v>
+      </c>
+      <c r="AA14" s="15">
+        <v>81</v>
+      </c>
+      <c r="AB14" s="14">
+        <v>-1</v>
+      </c>
+      <c r="AC14" s="16">
+        <v>5</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
@@ -1991,28 +2053,28 @@
       </c>
       <c r="H16">
         <f>MIN(H$3:H$14)</f>
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="J16" t="s">
         <v>14</v>
       </c>
       <c r="K16">
         <f>MIN(K$3:K$14)</f>
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="M16" t="s">
         <v>14</v>
       </c>
       <c r="N16">
         <f>MIN(N$3:N$14)</f>
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="P16" t="s">
         <v>14</v>
       </c>
       <c r="Q16">
         <f>MIN(Q$3:Q$14)</f>
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="S16" t="s">
         <v>14</v>
@@ -2099,11 +2161,11 @@
       </c>
       <c r="Y17">
         <f>MAX(Y$3:Y$14)</f>
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="Z17">
         <f>MAX(Z$3:Z$14)</f>
-        <v>16</v>
+        <v>600</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>15</v>
@@ -2121,126 +2183,126 @@
       <c r="G18" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <f>AVERAGE(H$3:H$14)</f>
-        <v>550.09090909090912</v>
+        <v>540.58333333333337</v>
       </c>
       <c r="J18" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="32">
+      <c r="K18" s="31">
         <f>AVERAGE(K$3:K$14)</f>
-        <v>455.45454545454544</v>
-      </c>
-      <c r="L18" s="33"/>
+        <v>453.83333333333331</v>
+      </c>
+      <c r="L18" s="32"/>
       <c r="M18" t="s">
         <v>16</v>
       </c>
-      <c r="N18" s="32">
+      <c r="N18" s="31">
         <f>AVERAGE(N$3:N$14)</f>
-        <v>468.63636363636363</v>
+        <v>465.91666666666669</v>
       </c>
       <c r="P18" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="32">
+      <c r="Q18" s="31">
         <f>AVERAGE(Q$3:Q$14)</f>
-        <v>462.18181818181819</v>
+        <v>460</v>
       </c>
       <c r="S18" t="s">
         <v>16</v>
       </c>
-      <c r="T18" s="32">
+      <c r="T18" s="31">
         <f>AVERAGE(T$3:T$14)</f>
         <v>485</v>
       </c>
       <c r="V18" t="s">
         <v>16</v>
       </c>
-      <c r="W18" s="32">
+      <c r="W18" s="31">
         <f>AVERAGE(W$3:W$14)</f>
         <v>600</v>
       </c>
       <c r="X18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Z18" s="32">
+      <c r="Z18" s="31">
         <f>AVERAGE(Z$3:Z$14)</f>
-        <v>-3.3636363636363638</v>
+        <v>46.916666666666664</v>
       </c>
       <c r="AA18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AB18" s="34">
+      <c r="AB18" s="33">
         <f>AVERAGE(AB$3:AB$14)</f>
-        <v>-0.45454545454545453</v>
-      </c>
-      <c r="AC18" s="32">
+        <v>-0.5</v>
+      </c>
+      <c r="AC18" s="31">
         <f>AVERAGE(AC$3:AC$14)</f>
-        <v>-3.6363636363636362</v>
+        <v>-2.9166666666666665</v>
       </c>
     </row>
     <row r="19" spans="7:29" x14ac:dyDescent="0.2">
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="31">
         <f>STDEV(H$3:H$14)</f>
-        <v>83.190690038554905</v>
+        <v>85.88518586761711</v>
       </c>
       <c r="J19" t="s">
         <v>17</v>
       </c>
-      <c r="K19" s="32">
+      <c r="K19" s="31">
         <f>STDEV(K$3:K$14)</f>
-        <v>14.801105609809264</v>
-      </c>
-      <c r="L19" s="33"/>
+        <v>15.188711916978665</v>
+      </c>
+      <c r="L19" s="32"/>
       <c r="M19" t="s">
         <v>17</v>
       </c>
-      <c r="N19" s="32">
+      <c r="N19" s="31">
         <f>STDEV(N$3:N$14)</f>
-        <v>24.146522429835429</v>
+        <v>24.875904125490717</v>
       </c>
       <c r="P19" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" s="32">
+      <c r="Q19" s="31">
         <f>STDEV(Q$3:Q$14)</f>
-        <v>19.843478434075926</v>
+        <v>20.373779941162343</v>
       </c>
       <c r="S19" t="s">
         <v>17</v>
       </c>
-      <c r="T19" s="32">
+      <c r="T19" s="31">
         <f>STDEV(T$3:T$14)</f>
         <v>0</v>
       </c>
       <c r="V19" t="s">
         <v>17</v>
       </c>
-      <c r="W19" s="32">
+      <c r="W19" s="31">
         <f>STDEV(W$3:W$14)</f>
         <v>0</v>
       </c>
       <c r="X19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z19" s="32">
+      <c r="Z19" s="31">
         <f>STDEV(Z$3:Z$14)</f>
-        <v>15.698870833742962</v>
+        <v>174.81806560137332</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB19" s="34">
+      <c r="AB19" s="33">
         <f>STDEV(AB$3:AB$14)</f>
-        <v>2.2962419891481978</v>
-      </c>
-      <c r="AC19" s="32">
+        <v>2.1950357213908429</v>
+      </c>
+      <c r="AC19" s="31">
         <f>STDEV(AC$3:AC$14)</f>
-        <v>15.207055778635963</v>
+        <v>14.712136816145019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-ran not-imputed w/ Strategy 8
</commit_message>
<xml_diff>
--- a/results/Strategies by Year Comparison.xlsx
+++ b/results/Strategies by Year Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A21026-F3E1-0046-B8DC-67153131A2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF81BBBC-4237-8C45-9F18-9B53A153A282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="17500" xr2:uid="{FDB991F3-65B7-2442-88EF-AF8858A1CE50}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -446,37 +446,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -803,7 +790,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD17" sqref="AD17"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,89 +1055,89 @@
       <c r="A4" s="11">
         <v>2002</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="3">
         <v>0.48270000000000002</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4">
         <v>205</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4">
         <v>434</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="1">
         <v>29</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4">
         <v>51</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4">
         <v>486</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="1">
         <v>8</v>
       </c>
-      <c r="J4" s="29">
+      <c r="J4">
         <v>8</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4">
         <v>443</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="1">
         <v>9</v>
       </c>
-      <c r="M4" s="29">
+      <c r="M4">
         <v>10</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4">
         <v>445</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="1">
         <v>9</v>
       </c>
-      <c r="P4" s="29">
+      <c r="P4">
         <v>10</v>
       </c>
-      <c r="Q4" s="29">
+      <c r="Q4">
         <f t="shared" ref="Q4:Q14" si="0">435+P4</f>
         <v>445</v>
       </c>
-      <c r="R4" s="30">
+      <c r="R4" s="1">
         <v>28</v>
       </c>
-      <c r="S4" s="29">
+      <c r="S4">
         <v>50</v>
       </c>
-      <c r="T4" s="29">
+      <c r="T4">
         <v>485</v>
       </c>
-      <c r="U4" s="30">
+      <c r="U4" s="1">
         <v>84</v>
       </c>
-      <c r="V4" s="29">
+      <c r="V4">
         <v>165</v>
       </c>
-      <c r="W4" s="29">
+      <c r="W4">
         <v>600</v>
       </c>
-      <c r="X4" s="30">
+      <c r="X4" s="1">
         <v>84</v>
       </c>
-      <c r="Y4" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="29">
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
         <v>10</v>
       </c>
-      <c r="AA4" s="30">
+      <c r="AA4" s="1">
         <v>85</v>
       </c>
-      <c r="AB4" s="29">
+      <c r="AB4">
         <v>-1</v>
       </c>
-      <c r="AC4" s="31">
+      <c r="AC4" s="28">
         <v>9</v>
       </c>
       <c r="AD4" t="s">
@@ -1161,89 +1148,89 @@
       <c r="A5" s="11">
         <v>2004</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="3">
         <v>0.4919</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5">
         <v>201</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5">
         <v>434</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5">
         <v>12</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="1">
         <v>44</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5">
         <v>65</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5">
         <v>500</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="1">
         <v>24</v>
       </c>
-      <c r="J5" s="29">
+      <c r="J5">
         <v>24</v>
       </c>
-      <c r="K5" s="29">
+      <c r="K5">
         <v>459</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="1">
         <v>28</v>
       </c>
-      <c r="M5" s="29">
+      <c r="M5">
         <v>32</v>
       </c>
-      <c r="N5" s="29">
+      <c r="N5">
         <v>467</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="1">
         <v>25</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5">
         <v>26</v>
       </c>
-      <c r="Q5" s="29">
+      <c r="Q5">
         <f t="shared" si="0"/>
         <v>461</v>
       </c>
-      <c r="R5" s="30">
+      <c r="R5" s="1">
         <v>37</v>
       </c>
-      <c r="S5" s="29">
+      <c r="S5">
         <v>50</v>
       </c>
-      <c r="T5" s="29">
+      <c r="T5">
         <v>485</v>
       </c>
-      <c r="U5" s="30">
+      <c r="U5" s="1">
         <v>93</v>
       </c>
-      <c r="V5" s="29">
+      <c r="V5">
         <v>165</v>
       </c>
-      <c r="W5" s="29">
+      <c r="W5">
         <v>600</v>
       </c>
-      <c r="X5" s="30">
+      <c r="X5" s="1">
         <v>93</v>
       </c>
-      <c r="Y5" s="29">
+      <c r="Y5">
         <v>1</v>
       </c>
-      <c r="Z5" s="29">
+      <c r="Z5">
         <v>5</v>
       </c>
-      <c r="AA5" s="30">
+      <c r="AA5" s="1">
         <v>94</v>
       </c>
-      <c r="AB5" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="31">
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="28">
         <v>4</v>
       </c>
       <c r="AD5" t="s">
@@ -1254,89 +1241,89 @@
       <c r="A6" s="11">
         <v>2006</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="3">
         <v>0.53520000000000001</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6">
         <v>233</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6">
         <v>435</v>
       </c>
-      <c r="E6" s="29">
-        <v>0</v>
-      </c>
-      <c r="F6" s="30">
-        <v>0</v>
-      </c>
-      <c r="G6" s="29">
-        <v>0</v>
-      </c>
-      <c r="H6" s="29">
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>435</v>
       </c>
-      <c r="I6" s="30">
-        <v>0</v>
-      </c>
-      <c r="J6" s="29">
-        <v>0</v>
-      </c>
-      <c r="K6" s="29">
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>435</v>
       </c>
-      <c r="L6" s="30">
-        <v>0</v>
-      </c>
-      <c r="M6" s="29">
-        <v>0</v>
-      </c>
-      <c r="N6" s="29">
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>435</v>
       </c>
-      <c r="O6" s="30">
-        <v>0</v>
-      </c>
-      <c r="P6" s="29">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="29">
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="0"/>
         <v>435</v>
       </c>
-      <c r="R6" s="30">
+      <c r="R6" s="1">
         <v>27</v>
       </c>
-      <c r="S6" s="29">
+      <c r="S6">
         <v>50</v>
       </c>
-      <c r="T6" s="29">
+      <c r="T6">
         <v>485</v>
       </c>
-      <c r="U6" s="30">
+      <c r="U6" s="1">
         <v>89</v>
       </c>
-      <c r="V6" s="29">
+      <c r="V6">
         <v>165</v>
       </c>
-      <c r="W6" s="29">
+      <c r="W6">
         <v>600</v>
       </c>
-      <c r="X6" s="30">
+      <c r="X6" s="1">
         <v>89</v>
       </c>
-      <c r="Y6" s="29">
+      <c r="Y6">
         <v>-1</v>
       </c>
-      <c r="Z6" s="29">
+      <c r="Z6">
         <v>-21</v>
       </c>
-      <c r="AA6" s="30">
+      <c r="AA6" s="1">
         <v>85</v>
       </c>
-      <c r="AB6" s="29">
+      <c r="AB6">
         <v>3</v>
       </c>
-      <c r="AC6" s="31">
+      <c r="AC6" s="28">
         <v>-17</v>
       </c>
       <c r="AD6" t="s">
@@ -1347,88 +1334,88 @@
       <c r="A7" s="11">
         <v>2008</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="3">
         <v>0.54679999999999995</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7">
         <v>257</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7">
         <v>435</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7">
         <v>-19</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="1">
         <v>54</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7">
         <v>133</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7">
         <v>568</v>
       </c>
-      <c r="I7" s="30">
-        <v>0</v>
-      </c>
-      <c r="J7" s="29">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>35</v>
       </c>
-      <c r="K7" s="29">
+      <c r="K7">
         <v>470</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="1">
         <v>7</v>
       </c>
-      <c r="M7" s="29">
+      <c r="M7">
         <v>47</v>
       </c>
-      <c r="N7" s="29">
+      <c r="N7">
         <v>482</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="1">
         <v>6</v>
       </c>
-      <c r="P7" s="29">
+      <c r="P7">
         <v>46</v>
       </c>
-      <c r="Q7" s="29">
+      <c r="Q7">
         <v>481</v>
       </c>
-      <c r="R7" s="30">
+      <c r="R7" s="1">
         <v>9</v>
       </c>
-      <c r="S7" s="29">
+      <c r="S7">
         <v>50</v>
       </c>
-      <c r="T7" s="29">
+      <c r="T7">
         <v>485</v>
       </c>
-      <c r="U7" s="30">
+      <c r="U7" s="1">
         <v>72</v>
       </c>
-      <c r="V7" s="29">
+      <c r="V7">
         <v>165</v>
       </c>
-      <c r="W7" s="29">
+      <c r="W7">
         <v>600</v>
       </c>
-      <c r="X7" s="30">
+      <c r="X7" s="1">
         <v>72</v>
       </c>
-      <c r="Y7" s="29">
+      <c r="Y7">
         <v>-1</v>
       </c>
-      <c r="Z7" s="29">
+      <c r="Z7">
         <v>-28</v>
       </c>
-      <c r="AA7" s="30">
+      <c r="AA7" s="1">
         <v>73</v>
       </c>
-      <c r="AB7" s="29">
+      <c r="AB7">
         <v>-2</v>
       </c>
-      <c r="AC7" s="31">
+      <c r="AC7" s="28">
         <v>-29</v>
       </c>
       <c r="AD7" t="s">
@@ -1439,89 +1426,89 @@
       <c r="A8" s="17">
         <v>2010</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>0.4723</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="30">
         <v>193</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="30">
         <v>435</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="30">
         <v>12</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="31">
         <v>54</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="30">
         <v>89</v>
       </c>
-      <c r="H8" s="33">
+      <c r="H8" s="30">
         <v>524</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="31">
         <v>23</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="30">
         <v>23</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="30">
         <v>458</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L8" s="31">
         <v>29</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="30">
         <v>36</v>
       </c>
-      <c r="N8" s="33">
+      <c r="N8" s="30">
         <v>471</v>
       </c>
-      <c r="O8" s="34">
+      <c r="O8" s="31">
         <v>28</v>
       </c>
-      <c r="P8" s="33">
+      <c r="P8" s="30">
         <v>33</v>
       </c>
-      <c r="Q8" s="33">
+      <c r="Q8" s="30">
         <f t="shared" si="0"/>
         <v>468</v>
       </c>
-      <c r="R8" s="34">
+      <c r="R8" s="31">
         <v>36</v>
       </c>
-      <c r="S8" s="33">
+      <c r="S8" s="30">
         <v>50</v>
       </c>
-      <c r="T8" s="33">
+      <c r="T8" s="30">
         <v>485</v>
       </c>
-      <c r="U8" s="34">
+      <c r="U8" s="31">
         <v>90</v>
       </c>
-      <c r="V8" s="33">
+      <c r="V8" s="30">
         <v>165</v>
       </c>
-      <c r="W8" s="33">
+      <c r="W8" s="30">
         <v>600</v>
       </c>
-      <c r="X8" s="34">
+      <c r="X8" s="31">
         <v>90</v>
       </c>
-      <c r="Y8" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="33">
+      <c r="Y8" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="30">
         <v>16</v>
       </c>
-      <c r="AA8" s="34">
+      <c r="AA8" s="31">
         <v>95</v>
       </c>
-      <c r="AB8" s="33">
+      <c r="AB8" s="30">
         <v>-5</v>
       </c>
-      <c r="AC8" s="35">
+      <c r="AC8" s="32">
         <v>11</v>
       </c>
       <c r="AD8"/>
@@ -1530,89 +1517,89 @@
       <c r="A9" s="21">
         <v>2012</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="3">
         <v>0.50849999999999995</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9">
         <v>201</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9">
         <v>435</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E9">
         <v>20</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="1">
         <v>106</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9">
         <v>169</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9">
         <v>604</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="1">
         <v>41</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9">
         <v>41</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9">
         <v>476</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="1">
         <v>54</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9">
         <v>67</v>
       </c>
-      <c r="N9" s="29">
+      <c r="N9">
         <v>502</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="1">
         <v>44</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9">
         <v>47</v>
       </c>
-      <c r="Q9" s="29">
+      <c r="Q9">
         <f t="shared" si="0"/>
         <v>482</v>
       </c>
-      <c r="R9" s="30">
+      <c r="R9" s="1">
         <v>46</v>
       </c>
-      <c r="S9" s="29">
+      <c r="S9">
         <v>50</v>
       </c>
-      <c r="T9" s="29">
+      <c r="T9">
         <v>485</v>
       </c>
-      <c r="U9" s="30">
+      <c r="U9" s="1">
         <v>105</v>
       </c>
-      <c r="V9" s="29">
+      <c r="V9">
         <v>165</v>
       </c>
-      <c r="W9" s="29">
+      <c r="W9">
         <v>600</v>
       </c>
-      <c r="X9" s="30">
+      <c r="X9" s="1">
         <v>105</v>
       </c>
-      <c r="Y9" s="29">
+      <c r="Y9">
         <v>-1</v>
       </c>
-      <c r="Z9" s="29">
+      <c r="Z9">
         <v>-5</v>
       </c>
-      <c r="AA9" s="30">
+      <c r="AA9" s="1">
         <v>102</v>
       </c>
-      <c r="AB9" s="29">
+      <c r="AB9">
         <v>2</v>
       </c>
-      <c r="AC9" s="31">
+      <c r="AC9" s="28">
         <v>-2</v>
       </c>
       <c r="AD9"/>
@@ -1621,89 +1608,89 @@
       <c r="A10" s="11">
         <v>2014</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="3">
         <v>0.47439999999999999</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10">
         <v>188</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10">
         <v>435</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10">
         <v>18</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="1">
         <v>88</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10">
         <v>147</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10">
         <v>582</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="1">
         <v>34</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10">
         <v>34</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10">
         <v>469</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="1">
         <v>50</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10">
         <v>67</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10">
         <v>502</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="1">
         <v>39</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10">
         <v>44</v>
       </c>
-      <c r="Q10" s="29">
+      <c r="Q10">
         <f t="shared" si="0"/>
         <v>479</v>
       </c>
-      <c r="R10" s="30">
+      <c r="R10" s="1">
         <v>42</v>
       </c>
-      <c r="S10" s="29">
+      <c r="S10">
         <v>50</v>
       </c>
-      <c r="T10" s="29">
+      <c r="T10">
         <v>485</v>
       </c>
-      <c r="U10" s="30">
+      <c r="U10" s="1">
         <v>96</v>
       </c>
-      <c r="V10" s="29">
+      <c r="V10">
         <v>165</v>
       </c>
-      <c r="W10" s="29">
+      <c r="W10">
         <v>600</v>
       </c>
-      <c r="X10" s="30">
+      <c r="X10" s="1">
         <v>96</v>
       </c>
-      <c r="Y10" s="29">
+      <c r="Y10">
         <v>1</v>
       </c>
-      <c r="Z10" s="29">
+      <c r="Z10">
         <v>15</v>
       </c>
-      <c r="AA10" s="30">
+      <c r="AA10" s="1">
         <v>95</v>
       </c>
-      <c r="AB10" s="29">
+      <c r="AB10">
         <v>2</v>
       </c>
-      <c r="AC10" s="31">
+      <c r="AC10" s="28">
         <v>16</v>
       </c>
       <c r="AD10"/>
@@ -1712,89 +1699,89 @@
       <c r="A11" s="11">
         <v>2016</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="3">
         <v>0.49530000000000002</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11">
         <v>194</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11">
         <v>435</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11">
         <v>21</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="1">
         <v>108</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11">
         <v>175</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11">
         <v>610</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="1">
         <v>42</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11">
         <v>42</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11">
         <v>477</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="1">
         <v>53</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11">
         <v>64</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11">
         <v>499</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="1">
         <v>46</v>
       </c>
-      <c r="P11" s="29">
+      <c r="P11">
         <v>50</v>
       </c>
-      <c r="Q11" s="29">
+      <c r="Q11">
         <f t="shared" si="0"/>
         <v>485</v>
       </c>
-      <c r="R11" s="30">
+      <c r="R11" s="1">
         <v>46</v>
       </c>
-      <c r="S11" s="29">
+      <c r="S11">
         <v>50</v>
       </c>
-      <c r="T11" s="29">
+      <c r="T11">
         <v>485</v>
       </c>
-      <c r="U11" s="30">
+      <c r="U11" s="1">
         <v>103</v>
       </c>
-      <c r="V11" s="29">
+      <c r="V11">
         <v>165</v>
       </c>
-      <c r="W11" s="29">
+      <c r="W11">
         <v>600</v>
       </c>
-      <c r="X11" s="30">
+      <c r="X11" s="1">
         <v>103</v>
       </c>
-      <c r="Y11" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="29">
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
         <v>2</v>
       </c>
-      <c r="AA11" s="30">
+      <c r="AA11" s="1">
         <v>101</v>
       </c>
-      <c r="AB11" s="29">
+      <c r="AB11">
         <v>2</v>
       </c>
-      <c r="AC11" s="31">
+      <c r="AC11" s="28">
         <v>4</v>
       </c>
       <c r="AD11"/>
@@ -1803,88 +1790,88 @@
       <c r="A12" s="11">
         <v>2018</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="3">
         <v>0.53539999999999999</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C12">
         <v>235</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12">
         <v>434</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E12">
         <v>-3</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="1">
         <v>42</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12">
         <v>83</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12">
         <v>518</v>
       </c>
-      <c r="I12" s="30">
-        <v>0</v>
-      </c>
-      <c r="J12" s="29">
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>4</v>
       </c>
-      <c r="K12" s="29">
+      <c r="K12">
         <v>439</v>
       </c>
-      <c r="L12" s="30">
+      <c r="L12" s="1">
         <v>5</v>
       </c>
-      <c r="M12" s="29">
+      <c r="M12">
         <v>14</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12">
         <v>449</v>
       </c>
-      <c r="O12" s="30">
+      <c r="O12" s="1">
         <v>3</v>
       </c>
-      <c r="P12" s="29">
+      <c r="P12">
         <v>10</v>
       </c>
-      <c r="Q12" s="29">
+      <c r="Q12">
         <v>445</v>
       </c>
-      <c r="R12" s="30">
+      <c r="R12" s="1">
         <v>25</v>
       </c>
-      <c r="S12" s="29">
+      <c r="S12">
         <v>50</v>
       </c>
-      <c r="T12" s="29">
+      <c r="T12">
         <v>485</v>
       </c>
-      <c r="U12" s="30">
+      <c r="U12" s="1">
         <v>86</v>
       </c>
-      <c r="V12" s="29">
+      <c r="V12">
         <v>165</v>
       </c>
-      <c r="W12" s="29">
+      <c r="W12">
         <v>600</v>
       </c>
-      <c r="X12" s="30">
+      <c r="X12" s="1">
         <v>86</v>
       </c>
-      <c r="Y12" s="29">
+      <c r="Y12">
         <v>-1</v>
       </c>
-      <c r="Z12" s="29">
+      <c r="Z12">
         <v>-21</v>
       </c>
-      <c r="AA12" s="30">
+      <c r="AA12" s="1">
         <v>87</v>
       </c>
-      <c r="AB12" s="29">
+      <c r="AB12">
         <v>-1</v>
       </c>
-      <c r="AC12" s="31">
+      <c r="AC12" s="28">
         <v>-22</v>
       </c>
       <c r="AD12" t="s">
@@ -1895,88 +1882,88 @@
       <c r="A13" s="17">
         <v>2020</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="29">
         <v>0.51080000000000003</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="30">
         <v>222</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="30">
         <v>435</v>
       </c>
-      <c r="E13" s="33">
-        <v>0</v>
-      </c>
-      <c r="F13" s="34">
-        <v>0</v>
-      </c>
-      <c r="G13" s="33">
-        <v>0</v>
-      </c>
-      <c r="H13" s="33">
+      <c r="E13" s="30">
+        <v>0</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0</v>
+      </c>
+      <c r="G13" s="30">
+        <v>0</v>
+      </c>
+      <c r="H13" s="30">
         <v>435</v>
       </c>
-      <c r="I13" s="34">
-        <v>0</v>
-      </c>
-      <c r="J13" s="33">
-        <v>0</v>
-      </c>
-      <c r="K13" s="33">
+      <c r="I13" s="31">
+        <v>0</v>
+      </c>
+      <c r="J13" s="30">
+        <v>0</v>
+      </c>
+      <c r="K13" s="30">
         <v>435</v>
       </c>
-      <c r="L13" s="34">
-        <v>0</v>
-      </c>
-      <c r="M13" s="33">
-        <v>0</v>
-      </c>
-      <c r="N13" s="33">
+      <c r="L13" s="31">
+        <v>0</v>
+      </c>
+      <c r="M13" s="30">
+        <v>0</v>
+      </c>
+      <c r="N13" s="30">
         <v>435</v>
       </c>
-      <c r="O13" s="34">
-        <v>0</v>
-      </c>
-      <c r="P13" s="33">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="33">
+      <c r="O13" s="31">
+        <v>0</v>
+      </c>
+      <c r="P13" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="30">
         <v>435</v>
       </c>
-      <c r="R13" s="34">
+      <c r="R13" s="31">
         <v>26</v>
       </c>
-      <c r="S13" s="33">
+      <c r="S13" s="30">
         <v>50</v>
       </c>
-      <c r="T13" s="33">
+      <c r="T13" s="30">
         <v>485</v>
       </c>
-      <c r="U13" s="34">
+      <c r="U13" s="31">
         <v>85</v>
       </c>
-      <c r="V13" s="33">
+      <c r="V13" s="30">
         <v>165</v>
       </c>
-      <c r="W13" s="33">
+      <c r="W13" s="30">
         <v>600</v>
       </c>
-      <c r="X13" s="34">
+      <c r="X13" s="31">
         <v>85</v>
       </c>
-      <c r="Y13" s="33">
+      <c r="Y13" s="30">
         <v>-1</v>
       </c>
-      <c r="Z13" s="33">
+      <c r="Z13" s="30">
         <v>-6</v>
       </c>
-      <c r="AA13" s="34">
+      <c r="AA13" s="31">
         <v>84</v>
       </c>
-      <c r="AB13" s="33">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="35">
+      <c r="AB13" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="32">
         <v>-5</v>
       </c>
       <c r="AD13"/>
@@ -1985,89 +1972,89 @@
       <c r="A14" s="23">
         <v>2022</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="33">
         <v>0.48809999999999998</v>
       </c>
-      <c r="C14" s="37">
+      <c r="C14" s="34">
         <v>213</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="34">
         <v>435</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="34">
         <v>-1</v>
       </c>
-      <c r="F14" s="38">
-        <v>0</v>
-      </c>
-      <c r="G14" s="37">
+      <c r="F14" s="35">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34">
         <v>1</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="34">
         <v>436</v>
       </c>
-      <c r="I14" s="38">
-        <v>0</v>
-      </c>
-      <c r="J14" s="37">
+      <c r="I14" s="35">
+        <v>0</v>
+      </c>
+      <c r="J14" s="34">
         <v>1</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="34">
         <v>436</v>
       </c>
-      <c r="L14" s="38">
-        <v>0</v>
-      </c>
-      <c r="M14" s="37">
+      <c r="L14" s="35">
+        <v>0</v>
+      </c>
+      <c r="M14" s="34">
         <v>1</v>
       </c>
-      <c r="N14" s="37">
+      <c r="N14" s="34">
         <v>436</v>
       </c>
-      <c r="O14" s="38">
-        <v>0</v>
-      </c>
-      <c r="P14" s="37">
+      <c r="O14" s="35">
+        <v>0</v>
+      </c>
+      <c r="P14" s="34">
         <v>1</v>
       </c>
-      <c r="Q14" s="37">
+      <c r="Q14" s="34">
         <f t="shared" si="0"/>
         <v>436</v>
       </c>
-      <c r="R14" s="38">
+      <c r="R14" s="35">
         <v>23</v>
       </c>
-      <c r="S14" s="37">
+      <c r="S14" s="34">
         <v>50</v>
       </c>
-      <c r="T14" s="37">
+      <c r="T14" s="34">
         <v>485</v>
       </c>
-      <c r="U14" s="38">
+      <c r="U14" s="35">
         <v>79</v>
       </c>
-      <c r="V14" s="37">
+      <c r="V14" s="34">
         <v>165</v>
       </c>
-      <c r="W14" s="37">
+      <c r="W14" s="34">
         <v>600</v>
       </c>
-      <c r="X14" s="38">
+      <c r="X14" s="35">
         <v>79</v>
       </c>
-      <c r="Y14" s="37">
+      <c r="Y14" s="34">
         <v>1</v>
       </c>
-      <c r="Z14" s="37">
+      <c r="Z14" s="34">
         <v>7</v>
       </c>
-      <c r="AA14" s="38">
+      <c r="AA14" s="35">
         <v>81</v>
       </c>
-      <c r="AB14" s="37">
+      <c r="AB14" s="34">
         <v>-1</v>
       </c>
-      <c r="AC14" s="39">
+      <c r="AC14" s="36">
         <v>5</v>
       </c>
       <c r="AD14" t="s">
@@ -2470,115 +2457,115 @@
       <c r="A23" s="11">
         <v>2002</v>
       </c>
-      <c r="B23" s="28">
+      <c r="B23" s="3">
         <f t="shared" ref="B23:AC23" si="2">B4-B37</f>
         <v>0</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H23" s="29">
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="30">
+      <c r="I23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K23" s="29">
+      <c r="K23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L23" s="30">
+      <c r="L23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M23" s="29">
+      <c r="M23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N23" s="29">
+      <c r="N23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="30">
+      <c r="O23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P23" s="29">
+      <c r="P23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="29">
+      <c r="Q23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R23" s="30">
+      <c r="R23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S23" s="29">
+      <c r="S23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T23" s="29">
+      <c r="T23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U23" s="30">
+      <c r="U23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V23" s="29">
+      <c r="V23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W23" s="29">
+      <c r="W23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X23" s="30">
+      <c r="X23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y23" s="29">
+      <c r="Y23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z23" s="29">
+      <c r="Z23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA23" s="30">
+      <c r="AA23" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB23" s="29">
+      <c r="AB23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC23" s="31">
+      <c r="AC23" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2587,115 +2574,115 @@
       <c r="A24" s="11">
         <v>2004</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="3">
         <f t="shared" ref="B24:AC24" si="3">B5-B38</f>
         <v>0</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L24" s="30">
+      <c r="L24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M24" s="29">
+      <c r="M24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N24" s="29">
+      <c r="N24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O24" s="30">
+      <c r="O24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P24" s="29">
+      <c r="P24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="29">
+      <c r="Q24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="R24" s="30">
+      <c r="R24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S24" s="29">
+      <c r="S24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T24" s="29">
+      <c r="T24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U24" s="30">
+      <c r="U24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="V24" s="29">
+      <c r="V24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="W24" s="29">
+      <c r="W24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="X24" s="30">
+      <c r="X24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Y24" s="29">
+      <c r="Y24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Z24" s="29">
+      <c r="Z24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AA24" s="30">
+      <c r="AA24" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB24" s="29">
+      <c r="AB24">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AC24" s="31">
+      <c r="AC24" s="28">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2704,115 +2691,115 @@
       <c r="A25" s="11">
         <v>2006</v>
       </c>
-      <c r="B25" s="28">
+      <c r="B25" s="3">
         <f t="shared" ref="B25:AC25" si="4">B6-B39</f>
         <v>-5.1999999999999824E-3</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="1">
         <f t="shared" si="4"/>
         <v>-167</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25">
         <f t="shared" si="4"/>
         <v>-306</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25">
         <f t="shared" si="4"/>
         <v>-306</v>
       </c>
-      <c r="I25" s="30">
+      <c r="I25" s="1">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="K25" s="29">
+      <c r="K25">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="L25" s="30">
+      <c r="L25" s="1">
         <f t="shared" si="4"/>
         <v>-5</v>
       </c>
-      <c r="M25" s="29">
+      <c r="M25">
         <f t="shared" si="4"/>
         <v>-6</v>
       </c>
-      <c r="N25" s="29">
+      <c r="N25">
         <f t="shared" si="4"/>
         <v>-6</v>
       </c>
-      <c r="O25" s="30">
+      <c r="O25" s="1">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="P25" s="29">
+      <c r="P25">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="Q25" s="29">
+      <c r="Q25">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="R25" s="30">
+      <c r="R25" s="1">
         <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-      <c r="S25" s="29">
+      <c r="S25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="T25" s="29">
+      <c r="T25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U25" s="30">
+      <c r="U25" s="1">
         <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-      <c r="V25" s="29">
+      <c r="V25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W25" s="29">
+      <c r="W25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X25" s="30">
+      <c r="X25" s="1">
         <f t="shared" si="4"/>
         <v>-3</v>
       </c>
-      <c r="Y25" s="29">
+      <c r="Y25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z25" s="29">
+      <c r="Z25">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="AA25" s="30">
+      <c r="AA25" s="1">
         <f t="shared" si="4"/>
         <v>-4</v>
       </c>
-      <c r="AB25" s="29">
+      <c r="AB25">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AC25" s="31">
+      <c r="AC25" s="28">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2821,115 +2808,115 @@
       <c r="A26" s="11">
         <v>2008</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="3">
         <f t="shared" ref="B26:AC26" si="5">B7-B40</f>
         <v>-6.0999999999999943E-3</v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="1">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="I26" s="30">
+      <c r="I26" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="K26" s="29">
+      <c r="K26">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="1">
         <f t="shared" si="5"/>
         <v>-2</v>
       </c>
-      <c r="M26" s="29">
+      <c r="M26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="N26" s="29">
+      <c r="N26">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="O26" s="30">
+      <c r="O26" s="1">
         <f t="shared" si="5"/>
         <v>-9</v>
       </c>
-      <c r="P26" s="29">
+      <c r="P26">
         <f t="shared" si="5"/>
         <v>-11</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="Q26">
         <f t="shared" si="5"/>
         <v>-11</v>
       </c>
-      <c r="R26" s="30">
+      <c r="R26" s="1">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="S26" s="29">
+      <c r="S26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="T26" s="29">
+      <c r="T26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="U26" s="30">
+      <c r="U26" s="1">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="V26" s="29">
+      <c r="V26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W26" s="29">
+      <c r="W26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="X26" s="30">
+      <c r="X26" s="1">
         <f t="shared" si="5"/>
         <v>-3</v>
       </c>
-      <c r="Y26" s="29">
+      <c r="Y26">
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
-      <c r="Z26" s="29">
+      <c r="Z26">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="AA26" s="30">
+      <c r="AA26" s="1">
         <f t="shared" si="5"/>
         <v>-4</v>
       </c>
-      <c r="AB26" s="29">
+      <c r="AB26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="31">
+      <c r="AC26" s="28">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -2938,115 +2925,115 @@
       <c r="A27" s="17">
         <v>2010</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B27" s="29">
         <f t="shared" ref="B27:AC27" si="6">B8-B41</f>
         <v>0</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F27" s="34">
+      <c r="F27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H27" s="33">
+      <c r="H27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K27" s="33">
+      <c r="K27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="L27" s="34">
+      <c r="L27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M27" s="33">
+      <c r="M27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="N27" s="33">
+      <c r="N27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="O27" s="34">
+      <c r="O27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P27" s="33">
+      <c r="P27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="33">
+      <c r="Q27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R27" s="34">
+      <c r="R27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="S27" s="33">
+      <c r="S27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="T27" s="33">
+      <c r="T27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="U27" s="34">
+      <c r="U27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V27" s="33">
+      <c r="V27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="W27" s="33">
+      <c r="W27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X27" s="34">
+      <c r="X27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Y27" s="33">
+      <c r="Y27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Z27" s="33">
+      <c r="Z27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AA27" s="34">
+      <c r="AA27" s="31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AB27" s="33">
+      <c r="AB27" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AC27" s="35">
+      <c r="AC27" s="32">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3055,115 +3042,115 @@
       <c r="A28" s="21">
         <v>2012</v>
       </c>
-      <c r="B28" s="28">
+      <c r="B28" s="3">
         <f t="shared" ref="B28:AC28" si="7">B9-B42</f>
         <v>0</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="H28" s="29">
+      <c r="H28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I28" s="30">
+      <c r="I28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J28" s="29">
+      <c r="J28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K28" s="29">
+      <c r="K28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="L28" s="30">
+      <c r="L28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M28" s="29">
+      <c r="M28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="N28" s="29">
+      <c r="N28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O28" s="30">
+      <c r="O28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P28" s="29">
+      <c r="P28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="29">
+      <c r="Q28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R28" s="30">
+      <c r="R28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S28" s="29">
+      <c r="S28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="T28" s="29">
+      <c r="T28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="U28" s="30">
+      <c r="U28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="V28" s="29">
+      <c r="V28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W28" s="29">
+      <c r="W28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="X28" s="30">
+      <c r="X28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y28" s="29">
+      <c r="Y28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Z28" s="29">
+      <c r="Z28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AA28" s="30">
+      <c r="AA28" s="1">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="29">
+      <c r="AB28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="31">
+      <c r="AC28" s="28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -3172,115 +3159,115 @@
       <c r="A29" s="11">
         <v>2014</v>
       </c>
-      <c r="B29" s="28">
+      <c r="B29" s="3">
         <f t="shared" ref="B29:AC29" si="8">B10-B43</f>
         <v>0</v>
       </c>
-      <c r="C29" s="29">
+      <c r="C29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H29" s="29">
+      <c r="H29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="I29" s="30">
+      <c r="I29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J29" s="29">
+      <c r="J29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K29" s="29">
+      <c r="K29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L29" s="30">
+      <c r="L29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M29" s="29">
+      <c r="M29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N29" s="29">
+      <c r="N29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O29" s="30">
+      <c r="O29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P29" s="29">
+      <c r="P29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="29">
+      <c r="Q29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="R29" s="30">
+      <c r="R29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S29" s="29">
+      <c r="S29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="T29" s="29">
+      <c r="T29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="U29" s="30">
+      <c r="U29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="V29" s="29">
+      <c r="V29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="W29" s="29">
+      <c r="W29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="X29" s="30">
+      <c r="X29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Y29" s="29">
+      <c r="Y29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z29" s="29">
+      <c r="Z29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AA29" s="30">
+      <c r="AA29" s="1">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="29">
+      <c r="AB29">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC29" s="31">
+      <c r="AC29" s="28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3289,115 +3276,115 @@
       <c r="A30" s="11">
         <v>2016</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="3">
         <f t="shared" ref="B30:AC30" si="9">B11-B44</f>
         <v>0</v>
       </c>
-      <c r="C30" s="29">
+      <c r="C30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G30" s="29">
+      <c r="G30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I30" s="30">
+      <c r="I30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J30" s="29">
+      <c r="J30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K30" s="29">
+      <c r="K30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="L30" s="30">
+      <c r="L30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="M30" s="29">
+      <c r="M30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N30" s="29">
+      <c r="N30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="O30" s="30">
+      <c r="O30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="P30" s="29">
+      <c r="P30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="29">
+      <c r="Q30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="R30" s="30">
+      <c r="R30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S30" s="29">
+      <c r="S30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="T30" s="29">
+      <c r="T30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="U30" s="30">
+      <c r="U30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="V30" s="29">
+      <c r="V30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="W30" s="29">
+      <c r="W30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="X30" s="30">
+      <c r="X30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Y30" s="29">
+      <c r="Y30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="Z30" s="29">
+      <c r="Z30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA30" s="30">
+      <c r="AA30" s="1">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="29">
+      <c r="AB30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AC30" s="31">
+      <c r="AC30" s="28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -3406,115 +3393,115 @@
       <c r="A31" s="11">
         <v>2018</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="3">
         <f t="shared" ref="B31:AC31" si="10">B12-B45</f>
         <v>2.0999999999999908E-3</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="1">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H31" s="29">
+      <c r="H31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I31" s="30">
+      <c r="I31" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="J31" s="29">
+      <c r="J31">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="K31" s="29">
+      <c r="K31">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="L31" s="30">
+      <c r="L31" s="1">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="M31" s="29">
+      <c r="M31">
         <f t="shared" si="10"/>
         <v>-5</v>
       </c>
-      <c r="N31" s="29">
+      <c r="N31">
         <f t="shared" si="10"/>
         <v>-5</v>
       </c>
-      <c r="O31" s="30">
+      <c r="O31" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="P31" s="29">
+      <c r="P31">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="Q31" s="29">
+      <c r="Q31">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
-      <c r="R31" s="30">
+      <c r="R31" s="1">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="S31" s="29">
+      <c r="S31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="T31" s="29">
+      <c r="T31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U31" s="30">
+      <c r="U31" s="1">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="V31" s="29">
+      <c r="V31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="W31" s="29">
+      <c r="W31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="X31" s="30">
+      <c r="X31" s="1">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Y31" s="29">
+      <c r="Y31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Z31" s="29">
+      <c r="Z31">
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="AA31" s="30">
+      <c r="AA31" s="1">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="AB31" s="29">
+      <c r="AB31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AC31" s="31">
+      <c r="AC31" s="28">
         <f t="shared" si="10"/>
         <v>-2</v>
       </c>
@@ -3523,115 +3510,115 @@
       <c r="A32" s="17">
         <v>2020</v>
       </c>
-      <c r="B32" s="32">
+      <c r="B32" s="29">
         <f t="shared" ref="B32:AC32" si="11">B13-B46</f>
         <v>4.0000000000000036E-3</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E32" s="30">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="31">
         <f t="shared" si="11"/>
         <v>-6</v>
       </c>
-      <c r="G32" s="33">
+      <c r="G32" s="30">
         <f t="shared" si="11"/>
         <v>-14</v>
       </c>
-      <c r="H32" s="33">
+      <c r="H32" s="30">
         <f t="shared" si="11"/>
         <v>-14</v>
       </c>
-      <c r="I32" s="34">
+      <c r="I32" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J32" s="33">
+      <c r="J32" s="30">
         <f t="shared" si="11"/>
         <v>-3</v>
       </c>
-      <c r="K32" s="33">
+      <c r="K32" s="30">
         <f t="shared" si="11"/>
         <v>-3</v>
       </c>
-      <c r="L32" s="34">
+      <c r="L32" s="31">
         <f t="shared" si="11"/>
         <v>-4</v>
       </c>
-      <c r="M32" s="33">
+      <c r="M32" s="30">
         <f t="shared" si="11"/>
         <v>-10</v>
       </c>
-      <c r="N32" s="33">
+      <c r="N32" s="30">
         <f t="shared" si="11"/>
         <v>-10</v>
       </c>
-      <c r="O32" s="34">
+      <c r="O32" s="31">
         <f t="shared" si="11"/>
         <v>-1</v>
       </c>
-      <c r="P32" s="33">
+      <c r="P32" s="30">
         <f t="shared" si="11"/>
         <v>-5</v>
       </c>
-      <c r="Q32" s="33">
+      <c r="Q32" s="30">
         <f t="shared" si="11"/>
         <v>-5</v>
       </c>
-      <c r="R32" s="34">
+      <c r="R32" s="31">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="S32" s="33">
+      <c r="S32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="T32" s="33">
+      <c r="T32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U32" s="34">
+      <c r="U32" s="31">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="V32" s="33">
+      <c r="V32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W32" s="33">
+      <c r="W32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X32" s="34">
+      <c r="X32" s="31">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="Y32" s="33">
+      <c r="Y32" s="30">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Z32" s="33">
+      <c r="Z32" s="30">
         <f t="shared" si="11"/>
         <v>-2</v>
       </c>
-      <c r="AA32" s="34">
+      <c r="AA32" s="31">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="33">
+      <c r="AB32" s="30">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="AC32" s="35">
+      <c r="AC32" s="32">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -3640,181 +3627,123 @@
       <c r="A33" s="23">
         <v>2022</v>
       </c>
-      <c r="B33" s="36">
+      <c r="B33" s="33">
         <f t="shared" ref="B33:AC33" si="12">B14-B47</f>
         <v>7.0999999999999952E-3</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="G33" s="37">
+      <c r="G33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="H33" s="37">
+      <c r="H33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J33" s="37">
+      <c r="J33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K33" s="37">
+      <c r="K33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="L33" s="38">
+      <c r="L33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M33" s="37">
+      <c r="M33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N33" s="37">
+      <c r="N33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="O33" s="38">
+      <c r="O33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="P33" s="37">
+      <c r="P33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="37">
+      <c r="Q33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="R33" s="38">
+      <c r="R33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="S33" s="37">
+      <c r="S33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="T33" s="37">
+      <c r="T33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="U33" s="38">
+      <c r="U33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="V33" s="37">
+      <c r="V33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="W33" s="37">
+      <c r="W33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X33" s="38">
+      <c r="X33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Y33" s="37">
+      <c r="Y33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="Z33" s="37">
+      <c r="Z33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AA33" s="38">
+      <c r="AA33" s="35">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AB33" s="37">
+      <c r="AB33" s="34">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AC33" s="39">
+      <c r="AC33" s="36">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="29"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="29"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="29"/>
-      <c r="T34" s="29"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="29"/>
-      <c r="W34" s="29"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="29"/>
-      <c r="Z34" s="29"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="29"/>
-      <c r="AC34" s="29"/>
     </row>
     <row r="35" spans="1:29" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="29"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="29"/>
-      <c r="R35" s="30"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="29"/>
-      <c r="W35" s="29"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="29"/>
-      <c r="Z35" s="29"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="29"/>
-      <c r="AC35" s="29"/>
     </row>
     <row r="36" spans="1:29" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
@@ -3909,88 +3838,88 @@
       <c r="A37" s="11">
         <v>2002</v>
       </c>
-      <c r="B37" s="28">
+      <c r="B37" s="3">
         <v>0.48270000000000002</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37">
         <v>205</v>
       </c>
-      <c r="D37" s="29">
+      <c r="D37">
         <v>434</v>
       </c>
-      <c r="E37" s="29">
+      <c r="E37">
         <v>4</v>
       </c>
-      <c r="F37" s="30">
+      <c r="F37" s="1">
         <v>29</v>
       </c>
-      <c r="G37" s="29">
+      <c r="G37">
         <v>51</v>
       </c>
-      <c r="H37" s="29">
+      <c r="H37">
         <v>486</v>
       </c>
-      <c r="I37" s="30">
+      <c r="I37" s="1">
         <v>8</v>
       </c>
-      <c r="J37" s="29">
+      <c r="J37">
         <v>8</v>
       </c>
-      <c r="K37" s="29">
+      <c r="K37">
         <v>443</v>
       </c>
-      <c r="L37" s="30">
+      <c r="L37" s="1">
         <v>9</v>
       </c>
-      <c r="M37" s="29">
+      <c r="M37">
         <v>10</v>
       </c>
-      <c r="N37" s="29">
+      <c r="N37">
         <v>445</v>
       </c>
-      <c r="O37" s="30">
+      <c r="O37" s="1">
         <v>9</v>
       </c>
-      <c r="P37" s="29">
+      <c r="P37">
         <v>10</v>
       </c>
-      <c r="Q37" s="29">
+      <c r="Q37">
         <v>445</v>
       </c>
-      <c r="R37" s="30">
+      <c r="R37" s="1">
         <v>28</v>
       </c>
-      <c r="S37" s="29">
+      <c r="S37">
         <v>50</v>
       </c>
-      <c r="T37" s="29">
+      <c r="T37">
         <v>485</v>
       </c>
-      <c r="U37" s="30">
+      <c r="U37" s="1">
         <v>84</v>
       </c>
-      <c r="V37" s="29">
+      <c r="V37">
         <v>165</v>
       </c>
-      <c r="W37" s="29">
+      <c r="W37">
         <v>600</v>
       </c>
-      <c r="X37" s="30">
+      <c r="X37" s="1">
         <v>84</v>
       </c>
-      <c r="Y37" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="29">
+      <c r="Y37">
+        <v>0</v>
+      </c>
+      <c r="Z37">
         <v>10</v>
       </c>
-      <c r="AA37" s="30">
+      <c r="AA37" s="1">
         <v>85</v>
       </c>
-      <c r="AB37" s="29">
+      <c r="AB37">
         <v>-1</v>
       </c>
-      <c r="AC37" s="31">
+      <c r="AC37" s="28">
         <v>9</v>
       </c>
     </row>
@@ -3998,88 +3927,88 @@
       <c r="A38" s="11">
         <v>2004</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="3">
         <v>0.4919</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C38">
         <v>201</v>
       </c>
-      <c r="D38" s="29">
+      <c r="D38">
         <v>434</v>
       </c>
-      <c r="E38" s="29">
+      <c r="E38">
         <v>12</v>
       </c>
-      <c r="F38" s="30">
+      <c r="F38" s="1">
         <v>44</v>
       </c>
-      <c r="G38" s="29">
+      <c r="G38">
         <v>65</v>
       </c>
-      <c r="H38" s="29">
+      <c r="H38">
         <v>500</v>
       </c>
-      <c r="I38" s="30">
+      <c r="I38" s="1">
         <v>24</v>
       </c>
-      <c r="J38" s="29">
+      <c r="J38">
         <v>24</v>
       </c>
-      <c r="K38" s="29">
+      <c r="K38">
         <v>459</v>
       </c>
-      <c r="L38" s="30">
+      <c r="L38" s="1">
         <v>28</v>
       </c>
-      <c r="M38" s="29">
+      <c r="M38">
         <v>32</v>
       </c>
-      <c r="N38" s="29">
+      <c r="N38">
         <v>467</v>
       </c>
-      <c r="O38" s="30">
+      <c r="O38" s="1">
         <v>25</v>
       </c>
-      <c r="P38" s="29">
+      <c r="P38">
         <v>26</v>
       </c>
-      <c r="Q38" s="29">
+      <c r="Q38">
         <v>461</v>
       </c>
-      <c r="R38" s="30">
+      <c r="R38" s="1">
         <v>37</v>
       </c>
-      <c r="S38" s="29">
+      <c r="S38">
         <v>50</v>
       </c>
-      <c r="T38" s="29">
+      <c r="T38">
         <v>485</v>
       </c>
-      <c r="U38" s="30">
+      <c r="U38" s="1">
         <v>93</v>
       </c>
-      <c r="V38" s="29">
+      <c r="V38">
         <v>165</v>
       </c>
-      <c r="W38" s="29">
+      <c r="W38">
         <v>600</v>
       </c>
-      <c r="X38" s="30">
+      <c r="X38" s="1">
         <v>93</v>
       </c>
-      <c r="Y38" s="29">
+      <c r="Y38">
         <v>1</v>
       </c>
-      <c r="Z38" s="29">
+      <c r="Z38">
         <v>5</v>
       </c>
-      <c r="AA38" s="30">
+      <c r="AA38" s="1">
         <v>94</v>
       </c>
-      <c r="AB38" s="29">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="31">
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="28">
         <v>4</v>
       </c>
     </row>
@@ -4087,88 +4016,88 @@
       <c r="A39" s="11">
         <v>2006</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="3">
         <v>0.54039999999999999</v>
       </c>
-      <c r="C39" s="29">
+      <c r="C39">
         <v>233</v>
       </c>
-      <c r="D39" s="29">
+      <c r="D39">
         <v>435</v>
       </c>
-      <c r="E39" s="29">
+      <c r="E39">
         <v>2</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="1">
         <v>167</v>
       </c>
-      <c r="G39" s="29">
+      <c r="G39">
         <v>306</v>
       </c>
-      <c r="H39" s="29">
+      <c r="H39">
         <v>741</v>
       </c>
-      <c r="I39" s="30">
+      <c r="I39" s="1">
         <v>4</v>
       </c>
-      <c r="J39" s="29">
+      <c r="J39">
         <v>4</v>
       </c>
-      <c r="K39" s="29">
+      <c r="K39">
         <v>439</v>
       </c>
-      <c r="L39" s="30">
+      <c r="L39" s="1">
         <v>5</v>
       </c>
-      <c r="M39" s="29">
+      <c r="M39">
         <v>6</v>
       </c>
-      <c r="N39" s="29">
+      <c r="N39">
         <v>441</v>
       </c>
-      <c r="O39" s="30">
+      <c r="O39" s="1">
         <v>4</v>
       </c>
-      <c r="P39" s="29">
+      <c r="P39">
         <v>4</v>
       </c>
-      <c r="Q39" s="29">
+      <c r="Q39">
         <v>439</v>
       </c>
-      <c r="R39" s="30">
+      <c r="R39" s="1">
         <v>30</v>
       </c>
-      <c r="S39" s="29">
+      <c r="S39">
         <v>50</v>
       </c>
-      <c r="T39" s="29">
+      <c r="T39">
         <v>485</v>
       </c>
-      <c r="U39" s="30">
+      <c r="U39" s="1">
         <v>92</v>
       </c>
-      <c r="V39" s="29">
+      <c r="V39">
         <v>165</v>
       </c>
-      <c r="W39" s="29">
+      <c r="W39">
         <v>600</v>
       </c>
-      <c r="X39" s="30">
+      <c r="X39" s="1">
         <v>92</v>
       </c>
-      <c r="Y39" s="29">
+      <c r="Y39">
         <v>-1</v>
       </c>
-      <c r="Z39" s="29">
+      <c r="Z39">
         <v>-24</v>
       </c>
-      <c r="AA39" s="30">
+      <c r="AA39" s="1">
         <v>89</v>
       </c>
-      <c r="AB39" s="29">
+      <c r="AB39">
         <v>2</v>
       </c>
-      <c r="AC39" s="31">
+      <c r="AC39" s="28">
         <v>-21</v>
       </c>
     </row>
@@ -4176,88 +4105,88 @@
       <c r="A40" s="11">
         <v>2008</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="3">
         <v>0.55289999999999995</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C40">
         <v>257</v>
       </c>
-      <c r="D40" s="29">
+      <c r="D40">
         <v>435</v>
       </c>
-      <c r="E40" s="29">
+      <c r="E40">
         <v>-16</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="1">
         <v>57</v>
       </c>
-      <c r="G40" s="29">
+      <c r="G40">
         <v>132</v>
       </c>
-      <c r="H40" s="29">
+      <c r="H40">
         <v>567</v>
       </c>
-      <c r="I40" s="30">
-        <v>0</v>
-      </c>
-      <c r="J40" s="29">
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40">
         <v>29</v>
       </c>
-      <c r="K40" s="29">
+      <c r="K40">
         <v>464</v>
       </c>
-      <c r="L40" s="30">
+      <c r="L40" s="1">
         <v>9</v>
       </c>
-      <c r="M40" s="29">
+      <c r="M40">
         <v>46</v>
       </c>
-      <c r="N40" s="29">
+      <c r="N40">
         <v>481</v>
       </c>
-      <c r="O40" s="30">
+      <c r="O40" s="1">
         <v>15</v>
       </c>
-      <c r="P40" s="29">
+      <c r="P40">
         <v>57</v>
       </c>
-      <c r="Q40" s="29">
+      <c r="Q40">
         <v>492</v>
       </c>
-      <c r="R40" s="30">
+      <c r="R40" s="1">
         <v>12</v>
       </c>
-      <c r="S40" s="29">
+      <c r="S40">
         <v>50</v>
       </c>
-      <c r="T40" s="29">
+      <c r="T40">
         <v>485</v>
       </c>
-      <c r="U40" s="30">
+      <c r="U40" s="1">
         <v>75</v>
       </c>
-      <c r="V40" s="29">
+      <c r="V40">
         <v>165</v>
       </c>
-      <c r="W40" s="29">
+      <c r="W40">
         <v>600</v>
       </c>
-      <c r="X40" s="30">
+      <c r="X40" s="1">
         <v>75</v>
       </c>
-      <c r="Y40" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="29">
+      <c r="Y40">
+        <v>0</v>
+      </c>
+      <c r="Z40">
         <v>-31</v>
       </c>
-      <c r="AA40" s="30">
+      <c r="AA40" s="1">
         <v>77</v>
       </c>
-      <c r="AB40" s="29">
+      <c r="AB40">
         <v>-2</v>
       </c>
-      <c r="AC40" s="31">
+      <c r="AC40" s="28">
         <v>-33</v>
       </c>
     </row>
@@ -4265,88 +4194,88 @@
       <c r="A41" s="17">
         <v>2010</v>
       </c>
-      <c r="B41" s="32">
+      <c r="B41" s="29">
         <v>0.4723</v>
       </c>
-      <c r="C41" s="33">
+      <c r="C41" s="30">
         <v>193</v>
       </c>
-      <c r="D41" s="33">
+      <c r="D41" s="30">
         <v>435</v>
       </c>
-      <c r="E41" s="33">
+      <c r="E41" s="30">
         <v>12</v>
       </c>
-      <c r="F41" s="34">
+      <c r="F41" s="31">
         <v>54</v>
       </c>
-      <c r="G41" s="33">
+      <c r="G41" s="30">
         <v>89</v>
       </c>
-      <c r="H41" s="33">
+      <c r="H41" s="30">
         <v>524</v>
       </c>
-      <c r="I41" s="34">
+      <c r="I41" s="31">
         <v>23</v>
       </c>
-      <c r="J41" s="33">
+      <c r="J41" s="30">
         <v>23</v>
       </c>
-      <c r="K41" s="33">
+      <c r="K41" s="30">
         <v>458</v>
       </c>
-      <c r="L41" s="34">
+      <c r="L41" s="31">
         <v>29</v>
       </c>
-      <c r="M41" s="33">
+      <c r="M41" s="30">
         <v>36</v>
       </c>
-      <c r="N41" s="33">
+      <c r="N41" s="30">
         <v>471</v>
       </c>
-      <c r="O41" s="34">
+      <c r="O41" s="31">
         <v>28</v>
       </c>
-      <c r="P41" s="33">
+      <c r="P41" s="30">
         <v>33</v>
       </c>
-      <c r="Q41" s="33">
+      <c r="Q41" s="30">
         <v>468</v>
       </c>
-      <c r="R41" s="34">
+      <c r="R41" s="31">
         <v>36</v>
       </c>
-      <c r="S41" s="33">
+      <c r="S41" s="30">
         <v>50</v>
       </c>
-      <c r="T41" s="33">
+      <c r="T41" s="30">
         <v>485</v>
       </c>
-      <c r="U41" s="34">
+      <c r="U41" s="31">
         <v>90</v>
       </c>
-      <c r="V41" s="33">
+      <c r="V41" s="30">
         <v>165</v>
       </c>
-      <c r="W41" s="33">
+      <c r="W41" s="30">
         <v>600</v>
       </c>
-      <c r="X41" s="34">
+      <c r="X41" s="31">
         <v>90</v>
       </c>
-      <c r="Y41" s="33">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="33">
+      <c r="Y41" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="30">
         <v>16</v>
       </c>
-      <c r="AA41" s="34">
+      <c r="AA41" s="31">
         <v>95</v>
       </c>
-      <c r="AB41" s="33">
+      <c r="AB41" s="30">
         <v>-5</v>
       </c>
-      <c r="AC41" s="35">
+      <c r="AC41" s="32">
         <v>11</v>
       </c>
     </row>
@@ -4354,88 +4283,88 @@
       <c r="A42" s="21">
         <v>2012</v>
       </c>
-      <c r="B42" s="28">
+      <c r="B42" s="3">
         <v>0.50849999999999995</v>
       </c>
-      <c r="C42" s="29">
+      <c r="C42">
         <v>201</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42">
         <v>435</v>
       </c>
-      <c r="E42" s="29">
+      <c r="E42">
         <v>20</v>
       </c>
-      <c r="F42" s="30">
+      <c r="F42" s="1">
         <v>106</v>
       </c>
-      <c r="G42" s="29">
+      <c r="G42">
         <v>169</v>
       </c>
-      <c r="H42" s="29">
+      <c r="H42">
         <v>604</v>
       </c>
-      <c r="I42" s="30">
+      <c r="I42" s="1">
         <v>41</v>
       </c>
-      <c r="J42" s="29">
+      <c r="J42">
         <v>41</v>
       </c>
-      <c r="K42" s="29">
+      <c r="K42">
         <v>476</v>
       </c>
-      <c r="L42" s="30">
+      <c r="L42" s="1">
         <v>54</v>
       </c>
-      <c r="M42" s="29">
+      <c r="M42">
         <v>67</v>
       </c>
-      <c r="N42" s="29">
+      <c r="N42">
         <v>502</v>
       </c>
-      <c r="O42" s="30">
+      <c r="O42" s="1">
         <v>44</v>
       </c>
-      <c r="P42" s="29">
+      <c r="P42">
         <v>47</v>
       </c>
-      <c r="Q42" s="29">
+      <c r="Q42">
         <v>482</v>
       </c>
-      <c r="R42" s="30">
+      <c r="R42" s="1">
         <v>46</v>
       </c>
-      <c r="S42" s="29">
+      <c r="S42">
         <v>50</v>
       </c>
-      <c r="T42" s="29">
+      <c r="T42">
         <v>485</v>
       </c>
-      <c r="U42" s="30">
+      <c r="U42" s="1">
         <v>105</v>
       </c>
-      <c r="V42" s="29">
+      <c r="V42">
         <v>165</v>
       </c>
-      <c r="W42" s="29">
+      <c r="W42">
         <v>600</v>
       </c>
-      <c r="X42" s="30">
+      <c r="X42" s="1">
         <v>105</v>
       </c>
-      <c r="Y42" s="29">
+      <c r="Y42">
         <v>-1</v>
       </c>
-      <c r="Z42" s="29">
+      <c r="Z42">
         <v>-5</v>
       </c>
-      <c r="AA42" s="30">
+      <c r="AA42" s="1">
         <v>102</v>
       </c>
-      <c r="AB42" s="29">
+      <c r="AB42">
         <v>2</v>
       </c>
-      <c r="AC42" s="31">
+      <c r="AC42" s="28">
         <v>-2</v>
       </c>
     </row>
@@ -4443,88 +4372,88 @@
       <c r="A43" s="11">
         <v>2014</v>
       </c>
-      <c r="B43" s="28">
+      <c r="B43" s="3">
         <v>0.47439999999999999</v>
       </c>
-      <c r="C43" s="29">
+      <c r="C43">
         <v>188</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D43">
         <v>435</v>
       </c>
-      <c r="E43" s="29">
+      <c r="E43">
         <v>18</v>
       </c>
-      <c r="F43" s="30">
+      <c r="F43" s="1">
         <v>88</v>
       </c>
-      <c r="G43" s="29">
+      <c r="G43">
         <v>147</v>
       </c>
-      <c r="H43" s="29">
+      <c r="H43">
         <v>582</v>
       </c>
-      <c r="I43" s="30">
+      <c r="I43" s="1">
         <v>34</v>
       </c>
-      <c r="J43" s="29">
+      <c r="J43">
         <v>34</v>
       </c>
-      <c r="K43" s="29">
+      <c r="K43">
         <v>469</v>
       </c>
-      <c r="L43" s="30">
+      <c r="L43" s="1">
         <v>50</v>
       </c>
-      <c r="M43" s="29">
+      <c r="M43">
         <v>67</v>
       </c>
-      <c r="N43" s="29">
+      <c r="N43">
         <v>502</v>
       </c>
-      <c r="O43" s="30">
+      <c r="O43" s="1">
         <v>39</v>
       </c>
-      <c r="P43" s="29">
+      <c r="P43">
         <v>44</v>
       </c>
-      <c r="Q43" s="29">
+      <c r="Q43">
         <v>479</v>
       </c>
-      <c r="R43" s="30">
+      <c r="R43" s="1">
         <v>42</v>
       </c>
-      <c r="S43" s="29">
+      <c r="S43">
         <v>50</v>
       </c>
-      <c r="T43" s="29">
+      <c r="T43">
         <v>485</v>
       </c>
-      <c r="U43" s="30">
+      <c r="U43" s="1">
         <v>96</v>
       </c>
-      <c r="V43" s="29">
+      <c r="V43">
         <v>165</v>
       </c>
-      <c r="W43" s="29">
+      <c r="W43">
         <v>600</v>
       </c>
-      <c r="X43" s="30">
+      <c r="X43" s="1">
         <v>96</v>
       </c>
-      <c r="Y43" s="29">
+      <c r="Y43">
         <v>1</v>
       </c>
-      <c r="Z43" s="29">
+      <c r="Z43">
         <v>15</v>
       </c>
-      <c r="AA43" s="30">
+      <c r="AA43" s="1">
         <v>95</v>
       </c>
-      <c r="AB43" s="29">
+      <c r="AB43">
         <v>2</v>
       </c>
-      <c r="AC43" s="31">
+      <c r="AC43" s="28">
         <v>16</v>
       </c>
     </row>
@@ -4532,88 +4461,88 @@
       <c r="A44" s="11">
         <v>2016</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B44" s="3">
         <v>0.49530000000000002</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44">
         <v>194</v>
       </c>
-      <c r="D44" s="29">
+      <c r="D44">
         <v>435</v>
       </c>
-      <c r="E44" s="29">
+      <c r="E44">
         <v>21</v>
       </c>
-      <c r="F44" s="30">
+      <c r="F44" s="1">
         <v>108</v>
       </c>
-      <c r="G44" s="29">
+      <c r="G44">
         <v>175</v>
       </c>
-      <c r="H44" s="29">
+      <c r="H44">
         <v>610</v>
       </c>
-      <c r="I44" s="30">
+      <c r="I44" s="1">
         <v>42</v>
       </c>
-      <c r="J44" s="29">
+      <c r="J44">
         <v>42</v>
       </c>
-      <c r="K44" s="29">
+      <c r="K44">
         <v>477</v>
       </c>
-      <c r="L44" s="30">
+      <c r="L44" s="1">
         <v>53</v>
       </c>
-      <c r="M44" s="29">
+      <c r="M44">
         <v>64</v>
       </c>
-      <c r="N44" s="29">
+      <c r="N44">
         <v>499</v>
       </c>
-      <c r="O44" s="30">
+      <c r="O44" s="1">
         <v>46</v>
       </c>
-      <c r="P44" s="29">
+      <c r="P44">
         <v>50</v>
       </c>
-      <c r="Q44" s="29">
+      <c r="Q44">
         <v>485</v>
       </c>
-      <c r="R44" s="30">
+      <c r="R44" s="1">
         <v>46</v>
       </c>
-      <c r="S44" s="29">
+      <c r="S44">
         <v>50</v>
       </c>
-      <c r="T44" s="29">
+      <c r="T44">
         <v>485</v>
       </c>
-      <c r="U44" s="30">
+      <c r="U44" s="1">
         <v>103</v>
       </c>
-      <c r="V44" s="29">
+      <c r="V44">
         <v>165</v>
       </c>
-      <c r="W44" s="29">
+      <c r="W44">
         <v>600</v>
       </c>
-      <c r="X44" s="30">
+      <c r="X44" s="1">
         <v>103</v>
       </c>
-      <c r="Y44" s="29">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="29">
+      <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
         <v>2</v>
       </c>
-      <c r="AA44" s="30">
+      <c r="AA44" s="1">
         <v>101</v>
       </c>
-      <c r="AB44" s="29">
+      <c r="AB44">
         <v>2</v>
       </c>
-      <c r="AC44" s="31">
+      <c r="AC44" s="28">
         <v>4</v>
       </c>
     </row>
@@ -4621,88 +4550,88 @@
       <c r="A45" s="11">
         <v>2018</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="3">
         <v>0.5333</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45">
         <v>235</v>
       </c>
-      <c r="D45" s="29">
+      <c r="D45">
         <v>434</v>
       </c>
-      <c r="E45" s="29">
+      <c r="E45">
         <v>-4</v>
       </c>
-      <c r="F45" s="30">
+      <c r="F45" s="1">
         <v>41</v>
       </c>
-      <c r="G45" s="29">
+      <c r="G45">
         <v>83</v>
       </c>
-      <c r="H45" s="29">
+      <c r="H45">
         <v>518</v>
       </c>
-      <c r="I45" s="30">
-        <v>0</v>
-      </c>
-      <c r="J45" s="29">
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="J45">
         <v>6</v>
       </c>
-      <c r="K45" s="29">
+      <c r="K45">
         <v>441</v>
       </c>
-      <c r="L45" s="30">
+      <c r="L45" s="1">
         <v>7</v>
       </c>
-      <c r="M45" s="29">
+      <c r="M45">
         <v>19</v>
       </c>
-      <c r="N45" s="29">
+      <c r="N45">
         <v>454</v>
       </c>
-      <c r="O45" s="30">
+      <c r="O45" s="1">
         <v>3</v>
       </c>
-      <c r="P45" s="29">
+      <c r="P45">
         <v>12</v>
       </c>
-      <c r="Q45" s="29">
+      <c r="Q45">
         <v>447</v>
       </c>
-      <c r="R45" s="30">
+      <c r="R45" s="1">
         <v>24</v>
       </c>
-      <c r="S45" s="29">
+      <c r="S45">
         <v>50</v>
       </c>
-      <c r="T45" s="29">
+      <c r="T45">
         <v>485</v>
       </c>
-      <c r="U45" s="30">
+      <c r="U45" s="1">
         <v>85</v>
       </c>
-      <c r="V45" s="29">
+      <c r="V45">
         <v>165</v>
       </c>
-      <c r="W45" s="29">
+      <c r="W45">
         <v>600</v>
       </c>
-      <c r="X45" s="30">
+      <c r="X45" s="1">
         <v>85</v>
       </c>
-      <c r="Y45" s="29">
+      <c r="Y45">
         <v>-1</v>
       </c>
-      <c r="Z45" s="29">
+      <c r="Z45">
         <v>-20</v>
       </c>
-      <c r="AA45" s="30">
+      <c r="AA45" s="1">
         <v>85</v>
       </c>
-      <c r="AB45" s="29">
+      <c r="AB45">
         <v>-1</v>
       </c>
-      <c r="AC45" s="31">
+      <c r="AC45" s="28">
         <v>-20</v>
       </c>
     </row>
@@ -4710,88 +4639,88 @@
       <c r="A46" s="17">
         <v>2020</v>
       </c>
-      <c r="B46" s="32">
+      <c r="B46" s="29">
         <v>0.50680000000000003</v>
       </c>
-      <c r="C46" s="33">
+      <c r="C46" s="30">
         <v>222</v>
       </c>
-      <c r="D46" s="33">
+      <c r="D46" s="30">
         <v>435</v>
       </c>
-      <c r="E46" s="33">
+      <c r="E46" s="30">
         <v>-2</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="31">
         <v>6</v>
       </c>
-      <c r="G46" s="33">
+      <c r="G46" s="30">
         <v>14</v>
       </c>
-      <c r="H46" s="33">
+      <c r="H46" s="30">
         <v>449</v>
       </c>
-      <c r="I46" s="34">
-        <v>0</v>
-      </c>
-      <c r="J46" s="33">
+      <c r="I46" s="31">
+        <v>0</v>
+      </c>
+      <c r="J46" s="30">
         <v>3</v>
       </c>
-      <c r="K46" s="33">
+      <c r="K46" s="30">
         <v>438</v>
       </c>
-      <c r="L46" s="34">
+      <c r="L46" s="31">
         <v>4</v>
       </c>
-      <c r="M46" s="33">
+      <c r="M46" s="30">
         <v>10</v>
       </c>
-      <c r="N46" s="33">
+      <c r="N46" s="30">
         <v>445</v>
       </c>
-      <c r="O46" s="34">
+      <c r="O46" s="31">
         <v>1</v>
       </c>
-      <c r="P46" s="33">
+      <c r="P46" s="30">
         <v>5</v>
       </c>
-      <c r="Q46" s="33">
+      <c r="Q46" s="30">
         <v>440</v>
       </c>
-      <c r="R46" s="34">
+      <c r="R46" s="31">
         <v>24</v>
       </c>
-      <c r="S46" s="33">
+      <c r="S46" s="30">
         <v>50</v>
       </c>
-      <c r="T46" s="33">
+      <c r="T46" s="30">
         <v>485</v>
       </c>
-      <c r="U46" s="34">
+      <c r="U46" s="31">
         <v>83</v>
       </c>
-      <c r="V46" s="33">
+      <c r="V46" s="30">
         <v>165</v>
       </c>
-      <c r="W46" s="33">
+      <c r="W46" s="30">
         <v>600</v>
       </c>
-      <c r="X46" s="34">
+      <c r="X46" s="31">
         <v>83</v>
       </c>
-      <c r="Y46" s="33">
+      <c r="Y46" s="30">
         <v>-1</v>
       </c>
-      <c r="Z46" s="33">
+      <c r="Z46" s="30">
         <v>-4</v>
       </c>
-      <c r="AA46" s="34">
+      <c r="AA46" s="31">
         <v>84</v>
       </c>
-      <c r="AB46" s="33">
+      <c r="AB46" s="30">
         <v>-2</v>
       </c>
-      <c r="AC46" s="35">
+      <c r="AC46" s="32">
         <v>-5</v>
       </c>
     </row>
@@ -4799,94 +4728,94 @@
       <c r="A47" s="23">
         <v>2022</v>
       </c>
-      <c r="B47" s="36">
+      <c r="B47" s="33">
         <v>0.48099999999999998</v>
       </c>
-      <c r="C47" s="37">
+      <c r="C47" s="34">
         <v>213</v>
       </c>
-      <c r="D47" s="37">
+      <c r="D47" s="34">
         <v>435</v>
       </c>
-      <c r="E47" s="37">
+      <c r="E47" s="34">
         <v>-1</v>
       </c>
-      <c r="F47" s="38">
-        <v>0</v>
-      </c>
-      <c r="G47" s="37">
+      <c r="F47" s="35">
+        <v>0</v>
+      </c>
+      <c r="G47" s="34">
         <v>1</v>
       </c>
-      <c r="H47" s="37">
+      <c r="H47" s="34">
         <v>436</v>
       </c>
-      <c r="I47" s="38">
-        <v>0</v>
-      </c>
-      <c r="J47" s="37">
+      <c r="I47" s="35">
+        <v>0</v>
+      </c>
+      <c r="J47" s="34">
         <v>1</v>
       </c>
-      <c r="K47" s="37">
+      <c r="K47" s="34">
         <v>436</v>
       </c>
-      <c r="L47" s="38">
-        <v>0</v>
-      </c>
-      <c r="M47" s="37">
+      <c r="L47" s="35">
+        <v>0</v>
+      </c>
+      <c r="M47" s="34">
         <v>1</v>
       </c>
-      <c r="N47" s="37">
+      <c r="N47" s="34">
         <v>436</v>
       </c>
-      <c r="O47" s="38">
-        <v>0</v>
-      </c>
-      <c r="P47" s="37">
+      <c r="O47" s="35">
+        <v>0</v>
+      </c>
+      <c r="P47" s="34">
         <v>1</v>
       </c>
-      <c r="Q47" s="37">
+      <c r="Q47" s="34">
         <v>436</v>
       </c>
-      <c r="R47" s="38">
+      <c r="R47" s="35">
         <v>23</v>
       </c>
-      <c r="S47" s="37">
+      <c r="S47" s="34">
         <v>50</v>
       </c>
-      <c r="T47" s="37">
+      <c r="T47" s="34">
         <v>485</v>
       </c>
-      <c r="U47" s="38">
+      <c r="U47" s="35">
         <v>79</v>
       </c>
-      <c r="V47" s="37">
+      <c r="V47" s="34">
         <v>165</v>
       </c>
-      <c r="W47" s="37">
+      <c r="W47" s="34">
         <v>600</v>
       </c>
-      <c r="X47" s="38">
+      <c r="X47" s="35">
         <v>79</v>
       </c>
-      <c r="Y47" s="37">
+      <c r="Y47" s="34">
         <v>1</v>
       </c>
-      <c r="Z47" s="37">
+      <c r="Z47" s="34">
         <v>7</v>
       </c>
-      <c r="AA47" s="38">
+      <c r="AA47" s="35">
         <v>81</v>
       </c>
-      <c r="AB47" s="37">
+      <c r="AB47" s="34">
         <v>-1</v>
       </c>
-      <c r="AC47" s="39">
+      <c r="AC47" s="36">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B22:AC33">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>B22&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>